<commit_message>
últimos test manuales del sprint 3
</commit_message>
<xml_diff>
--- a/Testing/Sprint 3/Casos-de-prueba/Documentacion-Testing-S3.xlsx
+++ b/Testing/Sprint 3/Casos-de-prueba/Documentacion-Testing-S3.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dina.perez.montes\Documents\Desde aquí\grupo-09\Testing\Sprint 3\Casos-de-prueba\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rainv\Desktop\Proyecto Integrador\Proyecto Entregable\grupo-09\Testing\Sprint 3\Casos-de-prueba\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E24EE1C5-C96B-4BE3-809B-745281B95E36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="28995" windowHeight="15675"/>
   </bookViews>
   <sheets>
     <sheet name="Casos de Prueba" sheetId="1" r:id="rId1"/>
@@ -30,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1808" uniqueCount="694">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1814" uniqueCount="693">
   <si>
     <t>ID</t>
   </si>
@@ -1949,9 +1948,6 @@
     <t>07/09/2022 - 12:14 pm</t>
   </si>
   <si>
-    <t>Se puede ver el form pero no me permite ingresar el dato de ciudad</t>
-  </si>
-  <si>
     <t>07/09/2022 - 12:44 pm</t>
   </si>
   <si>
@@ -2067,9 +2063,6 @@
     <t>ingresar en la web</t>
   </si>
   <si>
-    <t>Reportado</t>
-  </si>
-  <si>
     <t>Media</t>
   </si>
   <si>
@@ -2237,12 +2230,15 @@
   </si>
   <si>
     <t>Validar que cuando hace falta llenar un campo en el formulario no deje realizar la reserva</t>
+  </si>
+  <si>
+    <t>El mensaje de error no corresponde a la issue (resuelto el 07/09/2022)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
   </numFmts>
@@ -2867,47 +2863,26 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="22" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="21" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="5" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2916,38 +2891,53 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="5" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -2955,16 +2945,25 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2982,24 +2981,21 @@
     <xf numFmtId="0" fontId="14" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="22" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="21" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3212,74 +3208,74 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A129" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A84" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="8.59765625" customWidth="1"/>
-    <col min="2" max="2" width="12.46484375" customWidth="1"/>
-    <col min="3" max="3" width="22.59765625" customWidth="1"/>
-    <col min="4" max="4" width="46.46484375" customWidth="1"/>
-    <col min="5" max="5" width="12.46484375" customWidth="1"/>
-    <col min="6" max="6" width="17.46484375" customWidth="1"/>
-    <col min="7" max="7" width="6.1328125" customWidth="1"/>
-    <col min="8" max="8" width="36.46484375" customWidth="1"/>
+    <col min="1" max="1" width="8.5703125" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" customWidth="1"/>
+    <col min="3" max="3" width="22.5703125" customWidth="1"/>
+    <col min="4" max="4" width="46.42578125" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" customWidth="1"/>
+    <col min="7" max="7" width="6.140625" customWidth="1"/>
+    <col min="8" max="8" width="36.42578125" customWidth="1"/>
     <col min="9" max="9" width="54" customWidth="1"/>
-    <col min="10" max="10" width="12.46484375" customWidth="1"/>
-    <col min="11" max="11" width="17.46484375" customWidth="1"/>
-    <col min="12" max="26" width="12.46484375" customWidth="1"/>
+    <col min="10" max="10" width="12.42578125" customWidth="1"/>
+    <col min="11" max="11" width="17.42578125" customWidth="1"/>
+    <col min="12" max="26" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A1" s="72" t="s">
+      <c r="A1" s="76" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="72" t="s">
+      <c r="B1" s="76" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="72" t="s">
+      <c r="C1" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="72" t="s">
+      <c r="D1" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="72" t="s">
+      <c r="E1" s="76" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="72" t="s">
+      <c r="F1" s="76" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="73" t="s">
+      <c r="G1" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="74"/>
-      <c r="I1" s="75"/>
-      <c r="J1" s="72" t="s">
+      <c r="H1" s="71"/>
+      <c r="I1" s="72"/>
+      <c r="J1" s="76" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="72" t="s">
+      <c r="K1" s="76" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="72" t="s">
+      <c r="L1" s="76" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A2" s="69"/>
-      <c r="B2" s="69"/>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
-      <c r="F2" s="69"/>
+      <c r="A2" s="77"/>
+      <c r="B2" s="77"/>
+      <c r="C2" s="77"/>
+      <c r="D2" s="77"/>
+      <c r="E2" s="77"/>
+      <c r="F2" s="77"/>
       <c r="G2" s="1" t="s">
         <v>10</v>
       </c>
@@ -3289,25 +3285,25 @@
       <c r="I2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="69"/>
-      <c r="K2" s="69"/>
-      <c r="L2" s="69"/>
+      <c r="J2" s="77"/>
+      <c r="K2" s="77"/>
+      <c r="L2" s="77"/>
     </row>
     <row r="3" spans="1:13" ht="56.25" customHeight="1">
-      <c r="A3" s="76" t="s">
+      <c r="A3" s="75" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="74"/>
-      <c r="C3" s="74"/>
-      <c r="D3" s="74"/>
-      <c r="E3" s="74"/>
-      <c r="F3" s="74"/>
-      <c r="G3" s="74"/>
-      <c r="H3" s="74"/>
-      <c r="I3" s="74"/>
-      <c r="J3" s="74"/>
-      <c r="K3" s="74"/>
-      <c r="L3" s="75"/>
+      <c r="B3" s="71"/>
+      <c r="C3" s="71"/>
+      <c r="D3" s="71"/>
+      <c r="E3" s="71"/>
+      <c r="F3" s="71"/>
+      <c r="G3" s="71"/>
+      <c r="H3" s="71"/>
+      <c r="I3" s="71"/>
+      <c r="J3" s="71"/>
+      <c r="K3" s="71"/>
+      <c r="L3" s="72"/>
     </row>
     <row r="4" spans="1:13" ht="60.75" customHeight="1">
       <c r="A4" s="2" t="s">
@@ -3934,40 +3930,40 @@
       <c r="M19" s="4"/>
     </row>
     <row r="20" spans="1:26" ht="26.25" customHeight="1">
-      <c r="A20" s="63" t="s">
+      <c r="A20" s="66" t="s">
         <v>100</v>
       </c>
-      <c r="B20" s="80">
+      <c r="B20" s="69">
         <v>44779</v>
       </c>
-      <c r="C20" s="63" t="s">
+      <c r="C20" s="66" t="s">
         <v>101</v>
       </c>
-      <c r="D20" s="63" t="s">
+      <c r="D20" s="66" t="s">
         <v>102</v>
       </c>
-      <c r="E20" s="63" t="s">
+      <c r="E20" s="66" t="s">
         <v>80</v>
       </c>
-      <c r="F20" s="63" t="s">
+      <c r="F20" s="66" t="s">
         <v>103</v>
       </c>
-      <c r="G20" s="63">
+      <c r="G20" s="66">
         <v>1</v>
       </c>
-      <c r="H20" s="78" t="s">
+      <c r="H20" s="67" t="s">
         <v>104</v>
       </c>
-      <c r="I20" s="63" t="s">
+      <c r="I20" s="66" t="s">
         <v>105</v>
       </c>
-      <c r="J20" s="79" t="s">
+      <c r="J20" s="74" t="s">
         <v>21</v>
       </c>
-      <c r="K20" s="63" t="s">
+      <c r="K20" s="66" t="s">
         <v>106</v>
       </c>
-      <c r="L20" s="63" t="s">
+      <c r="L20" s="66" t="s">
         <v>107</v>
       </c>
       <c r="M20" s="6"/>
@@ -3986,18 +3982,18 @@
       <c r="Z20" s="6"/>
     </row>
     <row r="21" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A21" s="64"/>
-      <c r="B21" s="64"/>
-      <c r="C21" s="64"/>
-      <c r="D21" s="64"/>
-      <c r="E21" s="64"/>
-      <c r="F21" s="64"/>
-      <c r="G21" s="77"/>
-      <c r="H21" s="77"/>
-      <c r="I21" s="77"/>
-      <c r="J21" s="77"/>
-      <c r="K21" s="77"/>
-      <c r="L21" s="77"/>
+      <c r="A21" s="78"/>
+      <c r="B21" s="78"/>
+      <c r="C21" s="78"/>
+      <c r="D21" s="78"/>
+      <c r="E21" s="78"/>
+      <c r="F21" s="78"/>
+      <c r="G21" s="65"/>
+      <c r="H21" s="65"/>
+      <c r="I21" s="65"/>
+      <c r="J21" s="65"/>
+      <c r="K21" s="65"/>
+      <c r="L21" s="65"/>
       <c r="M21" s="6"/>
       <c r="N21" s="6"/>
       <c r="O21" s="6"/>
@@ -4014,12 +4010,12 @@
       <c r="Z21" s="6"/>
     </row>
     <row r="22" spans="1:26" ht="108.75" customHeight="1">
-      <c r="A22" s="77"/>
-      <c r="B22" s="77"/>
-      <c r="C22" s="77"/>
-      <c r="D22" s="77"/>
-      <c r="E22" s="77"/>
-      <c r="F22" s="77"/>
+      <c r="A22" s="65"/>
+      <c r="B22" s="65"/>
+      <c r="C22" s="65"/>
+      <c r="D22" s="65"/>
+      <c r="E22" s="65"/>
+      <c r="F22" s="65"/>
       <c r="G22" s="7">
         <v>2</v>
       </c>
@@ -4054,22 +4050,22 @@
       <c r="Z22" s="6"/>
     </row>
     <row r="23" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A23" s="63" t="s">
+      <c r="A23" s="66" t="s">
         <v>110</v>
       </c>
-      <c r="B23" s="80">
+      <c r="B23" s="69">
         <v>44779</v>
       </c>
-      <c r="C23" s="63" t="s">
+      <c r="C23" s="66" t="s">
         <v>111</v>
       </c>
-      <c r="D23" s="63" t="s">
+      <c r="D23" s="66" t="s">
         <v>112</v>
       </c>
-      <c r="E23" s="63" t="s">
+      <c r="E23" s="66" t="s">
         <v>17</v>
       </c>
-      <c r="F23" s="63" t="s">
+      <c r="F23" s="66" t="s">
         <v>113</v>
       </c>
       <c r="G23" s="7">
@@ -4078,16 +4074,16 @@
       <c r="H23" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="I23" s="63" t="s">
+      <c r="I23" s="66" t="s">
         <v>115</v>
       </c>
-      <c r="J23" s="79" t="s">
+      <c r="J23" s="74" t="s">
         <v>21</v>
       </c>
-      <c r="K23" s="63" t="s">
+      <c r="K23" s="66" t="s">
         <v>106</v>
       </c>
-      <c r="L23" s="63" t="s">
+      <c r="L23" s="66" t="s">
         <v>107</v>
       </c>
       <c r="M23" s="6"/>
@@ -4106,22 +4102,22 @@
       <c r="Z23" s="6"/>
     </row>
     <row r="24" spans="1:26" ht="71.25" customHeight="1">
-      <c r="A24" s="77"/>
-      <c r="B24" s="77"/>
-      <c r="C24" s="77"/>
-      <c r="D24" s="77"/>
-      <c r="E24" s="77"/>
-      <c r="F24" s="77"/>
+      <c r="A24" s="65"/>
+      <c r="B24" s="65"/>
+      <c r="C24" s="65"/>
+      <c r="D24" s="65"/>
+      <c r="E24" s="65"/>
+      <c r="F24" s="65"/>
       <c r="G24" s="7">
         <v>2</v>
       </c>
       <c r="H24" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="I24" s="77"/>
-      <c r="J24" s="77"/>
-      <c r="K24" s="77"/>
-      <c r="L24" s="77"/>
+      <c r="I24" s="65"/>
+      <c r="J24" s="65"/>
+      <c r="K24" s="65"/>
+      <c r="L24" s="65"/>
       <c r="M24" s="6"/>
       <c r="N24" s="6"/>
       <c r="O24" s="6"/>
@@ -4138,22 +4134,22 @@
       <c r="Z24" s="6"/>
     </row>
     <row r="25" spans="1:26" ht="48.75" customHeight="1">
-      <c r="A25" s="63" t="s">
+      <c r="A25" s="66" t="s">
         <v>117</v>
       </c>
-      <c r="B25" s="80">
+      <c r="B25" s="69">
         <v>44779</v>
       </c>
-      <c r="C25" s="78" t="s">
+      <c r="C25" s="67" t="s">
         <v>118</v>
       </c>
-      <c r="D25" s="78" t="s">
+      <c r="D25" s="67" t="s">
         <v>119</v>
       </c>
-      <c r="E25" s="78" t="s">
+      <c r="E25" s="67" t="s">
         <v>120</v>
       </c>
-      <c r="F25" s="78" t="s">
+      <c r="F25" s="67" t="s">
         <v>121</v>
       </c>
       <c r="G25" s="8">
@@ -4162,16 +4158,16 @@
       <c r="H25" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="I25" s="78" t="s">
+      <c r="I25" s="67" t="s">
         <v>123</v>
       </c>
-      <c r="J25" s="83" t="s">
+      <c r="J25" s="64" t="s">
         <v>21</v>
       </c>
-      <c r="K25" s="63" t="s">
+      <c r="K25" s="66" t="s">
         <v>22</v>
       </c>
-      <c r="L25" s="63" t="s">
+      <c r="L25" s="66" t="s">
         <v>107</v>
       </c>
       <c r="M25" s="6"/>
@@ -4190,22 +4186,22 @@
       <c r="Z25" s="6"/>
     </row>
     <row r="26" spans="1:26" ht="68.25" customHeight="1">
-      <c r="A26" s="77"/>
-      <c r="B26" s="77"/>
-      <c r="C26" s="77"/>
-      <c r="D26" s="77"/>
-      <c r="E26" s="77"/>
-      <c r="F26" s="77"/>
+      <c r="A26" s="65"/>
+      <c r="B26" s="65"/>
+      <c r="C26" s="65"/>
+      <c r="D26" s="65"/>
+      <c r="E26" s="65"/>
+      <c r="F26" s="65"/>
       <c r="G26" s="8">
         <v>2</v>
       </c>
       <c r="H26" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="I26" s="77"/>
-      <c r="J26" s="77"/>
-      <c r="K26" s="77"/>
-      <c r="L26" s="77"/>
+      <c r="I26" s="65"/>
+      <c r="J26" s="65"/>
+      <c r="K26" s="65"/>
+      <c r="L26" s="65"/>
       <c r="M26" s="6"/>
       <c r="N26" s="6"/>
       <c r="O26" s="6"/>
@@ -4222,22 +4218,22 @@
       <c r="Z26" s="6"/>
     </row>
     <row r="27" spans="1:26" ht="61.5" customHeight="1">
-      <c r="A27" s="63" t="s">
+      <c r="A27" s="66" t="s">
         <v>125</v>
       </c>
-      <c r="B27" s="80">
+      <c r="B27" s="69">
         <v>44779</v>
       </c>
-      <c r="C27" s="63" t="s">
+      <c r="C27" s="66" t="s">
         <v>126</v>
       </c>
-      <c r="D27" s="63" t="s">
+      <c r="D27" s="66" t="s">
         <v>127</v>
       </c>
-      <c r="E27" s="63" t="s">
+      <c r="E27" s="66" t="s">
         <v>17</v>
       </c>
-      <c r="F27" s="63" t="s">
+      <c r="F27" s="66" t="s">
         <v>128</v>
       </c>
       <c r="G27" s="7">
@@ -4246,13 +4242,13 @@
       <c r="H27" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="I27" s="63" t="s">
+      <c r="I27" s="66" t="s">
         <v>130</v>
       </c>
-      <c r="J27" s="83" t="s">
+      <c r="J27" s="64" t="s">
         <v>21</v>
       </c>
-      <c r="K27" s="63" t="s">
+      <c r="K27" s="66" t="s">
         <v>131</v>
       </c>
       <c r="L27" s="7" t="s">
@@ -4274,21 +4270,21 @@
       <c r="Z27" s="9"/>
     </row>
     <row r="28" spans="1:26" ht="128.25" customHeight="1">
-      <c r="A28" s="77"/>
-      <c r="B28" s="77"/>
-      <c r="C28" s="77"/>
-      <c r="D28" s="77"/>
-      <c r="E28" s="77"/>
-      <c r="F28" s="77"/>
+      <c r="A28" s="65"/>
+      <c r="B28" s="65"/>
+      <c r="C28" s="65"/>
+      <c r="D28" s="65"/>
+      <c r="E28" s="65"/>
+      <c r="F28" s="65"/>
       <c r="G28" s="7">
         <v>2</v>
       </c>
       <c r="H28" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="I28" s="77"/>
-      <c r="J28" s="77"/>
-      <c r="K28" s="77"/>
+      <c r="I28" s="65"/>
+      <c r="J28" s="65"/>
+      <c r="K28" s="65"/>
       <c r="L28" s="7" t="s">
         <v>133</v>
       </c>
@@ -4308,22 +4304,22 @@
       <c r="Z28" s="9"/>
     </row>
     <row r="29" spans="1:26" ht="56.25" customHeight="1">
-      <c r="A29" s="78" t="s">
+      <c r="A29" s="67" t="s">
         <v>134</v>
       </c>
-      <c r="B29" s="84">
+      <c r="B29" s="68">
         <v>44779</v>
       </c>
-      <c r="C29" s="78" t="s">
+      <c r="C29" s="67" t="s">
         <v>135</v>
       </c>
-      <c r="D29" s="78" t="s">
+      <c r="D29" s="67" t="s">
         <v>136</v>
       </c>
-      <c r="E29" s="78" t="s">
+      <c r="E29" s="67" t="s">
         <v>17</v>
       </c>
-      <c r="F29" s="78" t="s">
+      <c r="F29" s="67" t="s">
         <v>137</v>
       </c>
       <c r="G29" s="8" t="s">
@@ -4332,16 +4328,16 @@
       <c r="H29" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="I29" s="78" t="s">
+      <c r="I29" s="67" t="s">
         <v>140</v>
       </c>
-      <c r="J29" s="83" t="s">
+      <c r="J29" s="64" t="s">
         <v>21</v>
       </c>
-      <c r="K29" s="63" t="s">
+      <c r="K29" s="66" t="s">
         <v>22</v>
       </c>
-      <c r="L29" s="63" t="s">
+      <c r="L29" s="66" t="s">
         <v>141</v>
       </c>
       <c r="M29" s="9"/>
@@ -4360,22 +4356,22 @@
       <c r="Z29" s="9"/>
     </row>
     <row r="30" spans="1:26" ht="86.25" customHeight="1">
-      <c r="A30" s="77"/>
-      <c r="B30" s="77"/>
-      <c r="C30" s="77"/>
-      <c r="D30" s="77"/>
-      <c r="E30" s="77"/>
-      <c r="F30" s="77"/>
+      <c r="A30" s="65"/>
+      <c r="B30" s="65"/>
+      <c r="C30" s="65"/>
+      <c r="D30" s="65"/>
+      <c r="E30" s="65"/>
+      <c r="F30" s="65"/>
       <c r="G30" s="8" t="s">
         <v>142</v>
       </c>
       <c r="H30" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="I30" s="77"/>
-      <c r="J30" s="77"/>
-      <c r="K30" s="77"/>
-      <c r="L30" s="77"/>
+      <c r="I30" s="65"/>
+      <c r="J30" s="65"/>
+      <c r="K30" s="65"/>
+      <c r="L30" s="65"/>
       <c r="M30" s="9"/>
       <c r="N30" s="9"/>
       <c r="O30" s="9"/>
@@ -4392,22 +4388,22 @@
       <c r="Z30" s="9"/>
     </row>
     <row r="31" spans="1:26" ht="45" customHeight="1">
-      <c r="A31" s="63" t="s">
+      <c r="A31" s="66" t="s">
         <v>144</v>
       </c>
-      <c r="B31" s="80">
+      <c r="B31" s="69">
         <v>44779</v>
       </c>
-      <c r="C31" s="63" t="s">
+      <c r="C31" s="66" t="s">
         <v>145</v>
       </c>
-      <c r="D31" s="63" t="s">
+      <c r="D31" s="66" t="s">
         <v>146</v>
       </c>
-      <c r="E31" s="63" t="s">
+      <c r="E31" s="66" t="s">
         <v>17</v>
       </c>
-      <c r="F31" s="63" t="s">
+      <c r="F31" s="66" t="s">
         <v>147</v>
       </c>
       <c r="G31" s="7">
@@ -4416,16 +4412,16 @@
       <c r="H31" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="I31" s="63" t="s">
+      <c r="I31" s="66" t="s">
         <v>149</v>
       </c>
-      <c r="J31" s="83" t="s">
+      <c r="J31" s="64" t="s">
         <v>21</v>
       </c>
-      <c r="K31" s="63" t="s">
+      <c r="K31" s="66" t="s">
         <v>131</v>
       </c>
-      <c r="L31" s="63" t="s">
+      <c r="L31" s="66" t="s">
         <v>107</v>
       </c>
       <c r="M31" s="9"/>
@@ -4444,22 +4440,22 @@
       <c r="Z31" s="9"/>
     </row>
     <row r="32" spans="1:26" ht="54" customHeight="1">
-      <c r="A32" s="77"/>
-      <c r="B32" s="77"/>
-      <c r="C32" s="77"/>
-      <c r="D32" s="77"/>
-      <c r="E32" s="77"/>
-      <c r="F32" s="77"/>
+      <c r="A32" s="65"/>
+      <c r="B32" s="65"/>
+      <c r="C32" s="65"/>
+      <c r="D32" s="65"/>
+      <c r="E32" s="65"/>
+      <c r="F32" s="65"/>
       <c r="G32" s="7">
         <v>2</v>
       </c>
       <c r="H32" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="I32" s="77"/>
-      <c r="J32" s="77"/>
-      <c r="K32" s="77"/>
-      <c r="L32" s="77"/>
+      <c r="I32" s="65"/>
+      <c r="J32" s="65"/>
+      <c r="K32" s="65"/>
+      <c r="L32" s="65"/>
       <c r="M32" s="9"/>
       <c r="N32" s="9"/>
       <c r="O32" s="9"/>
@@ -4476,22 +4472,22 @@
       <c r="Z32" s="9"/>
     </row>
     <row r="33" spans="1:26" ht="76.5" customHeight="1">
-      <c r="A33" s="63" t="s">
+      <c r="A33" s="66" t="s">
         <v>151</v>
       </c>
-      <c r="B33" s="80">
+      <c r="B33" s="69">
         <v>44779</v>
       </c>
-      <c r="C33" s="63" t="s">
+      <c r="C33" s="66" t="s">
         <v>152</v>
       </c>
-      <c r="D33" s="63" t="s">
+      <c r="D33" s="66" t="s">
         <v>153</v>
       </c>
-      <c r="E33" s="63" t="s">
+      <c r="E33" s="66" t="s">
         <v>17</v>
       </c>
-      <c r="F33" s="63" t="s">
+      <c r="F33" s="66" t="s">
         <v>154</v>
       </c>
       <c r="G33" s="7" t="s">
@@ -4500,16 +4496,16 @@
       <c r="H33" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="I33" s="63" t="s">
+      <c r="I33" s="66" t="s">
         <v>156</v>
       </c>
-      <c r="J33" s="83" t="s">
+      <c r="J33" s="64" t="s">
         <v>21</v>
       </c>
-      <c r="K33" s="63" t="s">
+      <c r="K33" s="66" t="s">
         <v>131</v>
       </c>
-      <c r="L33" s="63" t="s">
+      <c r="L33" s="66" t="s">
         <v>107</v>
       </c>
       <c r="M33" s="9"/>
@@ -4528,22 +4524,22 @@
       <c r="Z33" s="9"/>
     </row>
     <row r="34" spans="1:26" ht="69" customHeight="1">
-      <c r="A34" s="77"/>
-      <c r="B34" s="77"/>
-      <c r="C34" s="77"/>
-      <c r="D34" s="77"/>
-      <c r="E34" s="77"/>
-      <c r="F34" s="77"/>
+      <c r="A34" s="65"/>
+      <c r="B34" s="65"/>
+      <c r="C34" s="65"/>
+      <c r="D34" s="65"/>
+      <c r="E34" s="65"/>
+      <c r="F34" s="65"/>
       <c r="G34" s="7" t="s">
         <v>142</v>
       </c>
       <c r="H34" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="I34" s="77"/>
-      <c r="J34" s="77"/>
-      <c r="K34" s="77"/>
-      <c r="L34" s="77"/>
+      <c r="I34" s="65"/>
+      <c r="J34" s="65"/>
+      <c r="K34" s="65"/>
+      <c r="L34" s="65"/>
       <c r="M34" s="9"/>
       <c r="N34" s="9"/>
       <c r="O34" s="9"/>
@@ -4560,22 +4556,22 @@
       <c r="Z34" s="9"/>
     </row>
     <row r="35" spans="1:26" ht="52.5" customHeight="1">
-      <c r="A35" s="78" t="s">
+      <c r="A35" s="67" t="s">
         <v>158</v>
       </c>
-      <c r="B35" s="84">
+      <c r="B35" s="68">
         <v>44779</v>
       </c>
-      <c r="C35" s="78" t="s">
+      <c r="C35" s="67" t="s">
         <v>159</v>
       </c>
-      <c r="D35" s="78" t="s">
+      <c r="D35" s="67" t="s">
         <v>160</v>
       </c>
-      <c r="E35" s="78" t="s">
+      <c r="E35" s="67" t="s">
         <v>17</v>
       </c>
-      <c r="F35" s="78" t="s">
+      <c r="F35" s="67" t="s">
         <v>161</v>
       </c>
       <c r="G35" s="8">
@@ -4584,16 +4580,16 @@
       <c r="H35" s="8" t="s">
         <v>162</v>
       </c>
-      <c r="I35" s="78" t="s">
+      <c r="I35" s="67" t="s">
         <v>163</v>
       </c>
-      <c r="J35" s="83" t="s">
+      <c r="J35" s="64" t="s">
         <v>21</v>
       </c>
-      <c r="K35" s="63" t="s">
+      <c r="K35" s="66" t="s">
         <v>131</v>
       </c>
-      <c r="L35" s="63" t="s">
+      <c r="L35" s="66" t="s">
         <v>141</v>
       </c>
       <c r="M35" s="9"/>
@@ -4612,22 +4608,22 @@
       <c r="Z35" s="9"/>
     </row>
     <row r="36" spans="1:26" ht="67.5" customHeight="1">
-      <c r="A36" s="77"/>
-      <c r="B36" s="77"/>
-      <c r="C36" s="77"/>
-      <c r="D36" s="77"/>
-      <c r="E36" s="77"/>
-      <c r="F36" s="77"/>
+      <c r="A36" s="65"/>
+      <c r="B36" s="65"/>
+      <c r="C36" s="65"/>
+      <c r="D36" s="65"/>
+      <c r="E36" s="65"/>
+      <c r="F36" s="65"/>
       <c r="G36" s="8">
         <v>2</v>
       </c>
       <c r="H36" s="10" t="s">
         <v>164</v>
       </c>
-      <c r="I36" s="77"/>
-      <c r="J36" s="77"/>
-      <c r="K36" s="77"/>
-      <c r="L36" s="77"/>
+      <c r="I36" s="65"/>
+      <c r="J36" s="65"/>
+      <c r="K36" s="65"/>
+      <c r="L36" s="65"/>
       <c r="M36" s="9"/>
       <c r="N36" s="9"/>
       <c r="O36" s="9"/>
@@ -4644,22 +4640,22 @@
       <c r="Z36" s="9"/>
     </row>
     <row r="37" spans="1:26" ht="60.75" customHeight="1">
-      <c r="A37" s="78" t="s">
+      <c r="A37" s="67" t="s">
         <v>165</v>
       </c>
-      <c r="B37" s="84">
+      <c r="B37" s="68">
         <v>44779</v>
       </c>
-      <c r="C37" s="78" t="s">
+      <c r="C37" s="67" t="s">
         <v>166</v>
       </c>
-      <c r="D37" s="78" t="s">
+      <c r="D37" s="67" t="s">
         <v>167</v>
       </c>
-      <c r="E37" s="78" t="s">
+      <c r="E37" s="67" t="s">
         <v>17</v>
       </c>
-      <c r="F37" s="78" t="s">
+      <c r="F37" s="67" t="s">
         <v>168</v>
       </c>
       <c r="G37" s="8">
@@ -4668,16 +4664,16 @@
       <c r="H37" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="I37" s="78" t="s">
+      <c r="I37" s="67" t="s">
         <v>170</v>
       </c>
-      <c r="J37" s="83" t="s">
+      <c r="J37" s="64" t="s">
         <v>21</v>
       </c>
-      <c r="K37" s="63" t="s">
+      <c r="K37" s="66" t="s">
         <v>131</v>
       </c>
-      <c r="L37" s="63" t="s">
+      <c r="L37" s="66" t="s">
         <v>107</v>
       </c>
       <c r="M37" s="9"/>
@@ -4696,22 +4692,22 @@
       <c r="Z37" s="9"/>
     </row>
     <row r="38" spans="1:26" ht="73.5" customHeight="1">
-      <c r="A38" s="77"/>
-      <c r="B38" s="77"/>
-      <c r="C38" s="77"/>
-      <c r="D38" s="77"/>
-      <c r="E38" s="77"/>
-      <c r="F38" s="77"/>
+      <c r="A38" s="65"/>
+      <c r="B38" s="65"/>
+      <c r="C38" s="65"/>
+      <c r="D38" s="65"/>
+      <c r="E38" s="65"/>
+      <c r="F38" s="65"/>
       <c r="G38" s="8">
         <v>2</v>
       </c>
       <c r="H38" s="8" t="s">
         <v>171</v>
       </c>
-      <c r="I38" s="77"/>
-      <c r="J38" s="77"/>
-      <c r="K38" s="77"/>
-      <c r="L38" s="77"/>
+      <c r="I38" s="65"/>
+      <c r="J38" s="65"/>
+      <c r="K38" s="65"/>
+      <c r="L38" s="65"/>
       <c r="M38" s="9"/>
       <c r="N38" s="9"/>
       <c r="O38" s="9"/>
@@ -4728,22 +4724,22 @@
       <c r="Z38" s="9"/>
     </row>
     <row r="39" spans="1:26" ht="60.75" customHeight="1">
-      <c r="A39" s="65" t="s">
+      <c r="A39" s="85" t="s">
         <v>172</v>
       </c>
-      <c r="B39" s="67">
+      <c r="B39" s="87">
         <v>44779</v>
       </c>
-      <c r="C39" s="65" t="s">
+      <c r="C39" s="85" t="s">
         <v>173</v>
       </c>
-      <c r="D39" s="65" t="s">
+      <c r="D39" s="85" t="s">
         <v>174</v>
       </c>
-      <c r="E39" s="65" t="s">
+      <c r="E39" s="85" t="s">
         <v>17</v>
       </c>
-      <c r="F39" s="65" t="s">
+      <c r="F39" s="85" t="s">
         <v>152</v>
       </c>
       <c r="G39" s="12">
@@ -4752,88 +4748,88 @@
       <c r="H39" s="12" t="s">
         <v>175</v>
       </c>
-      <c r="I39" s="65" t="s">
+      <c r="I39" s="85" t="s">
         <v>176</v>
       </c>
-      <c r="J39" s="61" t="s">
+      <c r="J39" s="83" t="s">
         <v>177</v>
       </c>
-      <c r="K39" s="63" t="s">
+      <c r="K39" s="66" t="s">
         <v>131</v>
       </c>
-      <c r="L39" s="63" t="s">
+      <c r="L39" s="66" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="40" spans="1:26" ht="72.75" customHeight="1">
-      <c r="A40" s="66"/>
-      <c r="B40" s="66"/>
-      <c r="C40" s="66"/>
-      <c r="D40" s="66"/>
-      <c r="E40" s="66"/>
-      <c r="F40" s="66"/>
+      <c r="A40" s="86"/>
+      <c r="B40" s="86"/>
+      <c r="C40" s="86"/>
+      <c r="D40" s="86"/>
+      <c r="E40" s="86"/>
+      <c r="F40" s="86"/>
       <c r="G40" s="11">
         <v>2</v>
       </c>
       <c r="H40" s="11" t="s">
         <v>178</v>
       </c>
-      <c r="I40" s="66"/>
-      <c r="J40" s="62"/>
-      <c r="K40" s="64"/>
-      <c r="L40" s="64"/>
+      <c r="I40" s="86"/>
+      <c r="J40" s="84"/>
+      <c r="K40" s="78"/>
+      <c r="L40" s="78"/>
     </row>
     <row r="41" spans="1:26" ht="38.25" customHeight="1">
-      <c r="A41" s="70" t="s">
+      <c r="A41" s="81" t="s">
         <v>179</v>
       </c>
-      <c r="B41" s="71">
+      <c r="B41" s="82">
         <v>44789</v>
       </c>
-      <c r="C41" s="68" t="s">
+      <c r="C41" s="80" t="s">
         <v>180</v>
       </c>
-      <c r="D41" s="68" t="s">
+      <c r="D41" s="80" t="s">
         <v>181</v>
       </c>
-      <c r="E41" s="68" t="s">
+      <c r="E41" s="80" t="s">
         <v>80</v>
       </c>
-      <c r="F41" s="68" t="s">
+      <c r="F41" s="80" t="s">
         <v>103</v>
       </c>
-      <c r="G41" s="68">
+      <c r="G41" s="80">
         <v>1</v>
       </c>
-      <c r="H41" s="68" t="s">
+      <c r="H41" s="80" t="s">
         <v>182</v>
       </c>
-      <c r="I41" s="68" t="s">
+      <c r="I41" s="80" t="s">
         <v>183</v>
       </c>
-      <c r="J41" s="68" t="s">
+      <c r="J41" s="80" t="s">
         <v>21</v>
       </c>
-      <c r="K41" s="68" t="s">
+      <c r="K41" s="80" t="s">
         <v>131</v>
       </c>
-      <c r="L41" s="68" t="s">
+      <c r="L41" s="80" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="42" spans="1:26" ht="76.5" customHeight="1">
-      <c r="A42" s="69"/>
-      <c r="B42" s="69"/>
-      <c r="C42" s="69"/>
-      <c r="D42" s="69"/>
-      <c r="E42" s="69"/>
-      <c r="F42" s="69"/>
-      <c r="G42" s="69"/>
-      <c r="H42" s="69"/>
-      <c r="I42" s="69"/>
-      <c r="J42" s="69"/>
-      <c r="K42" s="69"/>
-      <c r="L42" s="69"/>
+      <c r="A42" s="77"/>
+      <c r="B42" s="77"/>
+      <c r="C42" s="77"/>
+      <c r="D42" s="77"/>
+      <c r="E42" s="77"/>
+      <c r="F42" s="77"/>
+      <c r="G42" s="77"/>
+      <c r="H42" s="77"/>
+      <c r="I42" s="77"/>
+      <c r="J42" s="77"/>
+      <c r="K42" s="77"/>
+      <c r="L42" s="77"/>
     </row>
     <row r="43" spans="1:26" ht="67.5" customHeight="1">
       <c r="A43" s="13" t="s">
@@ -4926,20 +4922,20 @@
       <c r="L45" s="15"/>
     </row>
     <row r="46" spans="1:26" ht="49.5" customHeight="1">
-      <c r="A46" s="81" t="s">
+      <c r="A46" s="70" t="s">
         <v>193</v>
       </c>
-      <c r="B46" s="74"/>
-      <c r="C46" s="74"/>
-      <c r="D46" s="74"/>
-      <c r="E46" s="74"/>
-      <c r="F46" s="74"/>
-      <c r="G46" s="74"/>
-      <c r="H46" s="74"/>
-      <c r="I46" s="74"/>
-      <c r="J46" s="74"/>
-      <c r="K46" s="74"/>
-      <c r="L46" s="75"/>
+      <c r="B46" s="71"/>
+      <c r="C46" s="71"/>
+      <c r="D46" s="71"/>
+      <c r="E46" s="71"/>
+      <c r="F46" s="71"/>
+      <c r="G46" s="71"/>
+      <c r="H46" s="71"/>
+      <c r="I46" s="71"/>
+      <c r="J46" s="71"/>
+      <c r="K46" s="71"/>
+      <c r="L46" s="72"/>
     </row>
     <row r="47" spans="1:26" ht="113.25" customHeight="1">
       <c r="A47" s="17" t="s">
@@ -6343,7 +6339,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="85" spans="1:12" ht="89.25">
+    <row r="85" spans="1:12" ht="102">
       <c r="A85" s="17" t="s">
         <v>361</v>
       </c>
@@ -6410,20 +6406,20 @@
       <c r="L87" s="15"/>
     </row>
     <row r="88" spans="1:12" ht="47.25" customHeight="1">
-      <c r="A88" s="82" t="s">
+      <c r="A88" s="73" t="s">
         <v>369</v>
       </c>
-      <c r="B88" s="74"/>
-      <c r="C88" s="74"/>
-      <c r="D88" s="74"/>
-      <c r="E88" s="74"/>
-      <c r="F88" s="74"/>
-      <c r="G88" s="74"/>
-      <c r="H88" s="74"/>
-      <c r="I88" s="74"/>
-      <c r="J88" s="74"/>
-      <c r="K88" s="74"/>
-      <c r="L88" s="75"/>
+      <c r="B88" s="71"/>
+      <c r="C88" s="71"/>
+      <c r="D88" s="71"/>
+      <c r="E88" s="71"/>
+      <c r="F88" s="71"/>
+      <c r="G88" s="71"/>
+      <c r="H88" s="71"/>
+      <c r="I88" s="71"/>
+      <c r="J88" s="71"/>
+      <c r="K88" s="71"/>
+      <c r="L88" s="72"/>
     </row>
     <row r="89" spans="1:12" ht="84" customHeight="1">
       <c r="A89" s="13" t="s">
@@ -19981,53 +19977,61 @@
     </row>
   </sheetData>
   <mergeCells count="126">
-    <mergeCell ref="J37:J38"/>
-    <mergeCell ref="K37:K38"/>
-    <mergeCell ref="L37:L38"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="F37:F38"/>
-    <mergeCell ref="I37:I38"/>
-    <mergeCell ref="J35:J36"/>
-    <mergeCell ref="K35:K36"/>
-    <mergeCell ref="L35:L36"/>
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="E35:E36"/>
-    <mergeCell ref="F35:F36"/>
-    <mergeCell ref="I35:I36"/>
-    <mergeCell ref="L31:L32"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="F31:F32"/>
-    <mergeCell ref="I31:I32"/>
-    <mergeCell ref="J33:J34"/>
-    <mergeCell ref="K33:K34"/>
-    <mergeCell ref="L33:L34"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="E33:E34"/>
-    <mergeCell ref="F33:F34"/>
-    <mergeCell ref="I33:I34"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="F29:F30"/>
-    <mergeCell ref="I29:I30"/>
-    <mergeCell ref="J31:J32"/>
-    <mergeCell ref="K31:K32"/>
+    <mergeCell ref="J39:J40"/>
+    <mergeCell ref="K39:K40"/>
+    <mergeCell ref="L39:L40"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="E39:E40"/>
+    <mergeCell ref="F39:F40"/>
+    <mergeCell ref="I39:I40"/>
+    <mergeCell ref="H41:H42"/>
+    <mergeCell ref="I41:I42"/>
+    <mergeCell ref="J41:J42"/>
+    <mergeCell ref="K41:K42"/>
+    <mergeCell ref="L41:L42"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="E41:E42"/>
+    <mergeCell ref="F41:F42"/>
+    <mergeCell ref="G41:G42"/>
+    <mergeCell ref="A3:L3"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="H20:H21"/>
+    <mergeCell ref="I20:I21"/>
+    <mergeCell ref="J20:J21"/>
+    <mergeCell ref="K20:K21"/>
+    <mergeCell ref="L20:L21"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="D20:D22"/>
+    <mergeCell ref="E20:E22"/>
+    <mergeCell ref="F20:F22"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="J23:J24"/>
+    <mergeCell ref="K23:K24"/>
+    <mergeCell ref="L23:L24"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="I23:I24"/>
     <mergeCell ref="A46:L46"/>
     <mergeCell ref="A88:L88"/>
     <mergeCell ref="J25:J26"/>
@@ -20052,64 +20056,56 @@
     <mergeCell ref="J29:J30"/>
     <mergeCell ref="K29:K30"/>
     <mergeCell ref="L29:L30"/>
-    <mergeCell ref="J23:J24"/>
-    <mergeCell ref="K23:K24"/>
-    <mergeCell ref="L23:L24"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="F23:F24"/>
-    <mergeCell ref="I23:I24"/>
-    <mergeCell ref="A3:L3"/>
-    <mergeCell ref="G20:G21"/>
-    <mergeCell ref="H20:H21"/>
-    <mergeCell ref="I20:I21"/>
-    <mergeCell ref="J20:J21"/>
-    <mergeCell ref="K20:K21"/>
-    <mergeCell ref="L20:L21"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="A20:A22"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="D20:D22"/>
-    <mergeCell ref="E20:E22"/>
-    <mergeCell ref="F20:F22"/>
-    <mergeCell ref="J1:J2"/>
-    <mergeCell ref="K1:K2"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="H41:H42"/>
-    <mergeCell ref="I41:I42"/>
-    <mergeCell ref="J41:J42"/>
-    <mergeCell ref="K41:K42"/>
-    <mergeCell ref="L41:L42"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="D41:D42"/>
-    <mergeCell ref="E41:E42"/>
-    <mergeCell ref="F41:F42"/>
-    <mergeCell ref="G41:G42"/>
-    <mergeCell ref="J39:J40"/>
-    <mergeCell ref="K39:K40"/>
-    <mergeCell ref="L39:L40"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="C39:C40"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="E39:E40"/>
-    <mergeCell ref="F39:F40"/>
-    <mergeCell ref="I39:I40"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="I29:I30"/>
+    <mergeCell ref="J31:J32"/>
+    <mergeCell ref="K31:K32"/>
+    <mergeCell ref="L31:L32"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="F31:F32"/>
+    <mergeCell ref="I31:I32"/>
+    <mergeCell ref="J33:J34"/>
+    <mergeCell ref="K33:K34"/>
+    <mergeCell ref="L33:L34"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="F33:F34"/>
+    <mergeCell ref="I33:I34"/>
+    <mergeCell ref="J35:J36"/>
+    <mergeCell ref="K35:K36"/>
+    <mergeCell ref="L35:L36"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="E35:E36"/>
+    <mergeCell ref="F35:F36"/>
+    <mergeCell ref="I35:I36"/>
+    <mergeCell ref="J37:J38"/>
+    <mergeCell ref="K37:K38"/>
+    <mergeCell ref="L37:L38"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="F37:F38"/>
+    <mergeCell ref="I37:I38"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="H36" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="H36" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
@@ -20117,7 +20113,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -20125,15 +20121,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="30" customWidth="1"/>
-    <col min="2" max="2" width="34.3984375" customWidth="1"/>
-    <col min="3" max="3" width="25.3984375" customWidth="1"/>
-    <col min="4" max="4" width="25.46484375" customWidth="1"/>
-    <col min="5" max="5" width="21.1328125" customWidth="1"/>
-    <col min="6" max="6" width="20.3984375" customWidth="1"/>
-    <col min="7" max="26" width="12.46484375" customWidth="1"/>
+    <col min="2" max="2" width="34.42578125" customWidth="1"/>
+    <col min="3" max="4" width="25.42578125" customWidth="1"/>
+    <col min="5" max="5" width="21.140625" customWidth="1"/>
+    <col min="6" max="6" width="20.42578125" customWidth="1"/>
+    <col min="7" max="26" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="30" customHeight="1">
@@ -30435,7 +30430,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -30443,15 +30438,15 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="17.3984375" customWidth="1"/>
-    <col min="2" max="2" width="29.46484375" customWidth="1"/>
-    <col min="3" max="3" width="30.3984375" customWidth="1"/>
-    <col min="4" max="4" width="26.1328125" customWidth="1"/>
-    <col min="5" max="5" width="24.46484375" customWidth="1"/>
+    <col min="1" max="1" width="17.42578125" customWidth="1"/>
+    <col min="2" max="2" width="29.42578125" customWidth="1"/>
+    <col min="3" max="3" width="30.42578125" customWidth="1"/>
+    <col min="4" max="4" width="26.140625" customWidth="1"/>
+    <col min="5" max="5" width="24.42578125" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
-    <col min="7" max="26" width="12.46484375" customWidth="1"/>
+    <col min="7" max="26" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="36" customHeight="1">
@@ -40939,26 +40934,26 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:H1001"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3:B4"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="20.46484375" customWidth="1"/>
-    <col min="2" max="2" width="10.1328125" customWidth="1"/>
-    <col min="3" max="3" width="12.46484375" customWidth="1"/>
-    <col min="4" max="4" width="26.59765625" customWidth="1"/>
-    <col min="5" max="5" width="26.46484375" customWidth="1"/>
-    <col min="6" max="6" width="27.46484375" customWidth="1"/>
-    <col min="7" max="7" width="18.1328125" customWidth="1"/>
+    <col min="1" max="1" width="20.42578125" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" customWidth="1"/>
+    <col min="4" max="4" width="26.5703125" customWidth="1"/>
+    <col min="5" max="5" width="26.42578125" customWidth="1"/>
+    <col min="6" max="6" width="27.42578125" customWidth="1"/>
+    <col min="7" max="7" width="18.140625" customWidth="1"/>
     <col min="8" max="8" width="43" customWidth="1"/>
   </cols>
   <sheetData>
@@ -41011,38 +41006,38 @@
       <c r="H2" s="44"/>
     </row>
     <row r="3" spans="1:8" ht="33" customHeight="1">
-      <c r="A3" s="85">
+      <c r="A3" s="89">
         <v>44798</v>
       </c>
-      <c r="B3" s="86" t="s">
+      <c r="B3" s="88" t="s">
         <v>378</v>
       </c>
-      <c r="C3" s="86" t="s">
+      <c r="C3" s="88" t="s">
         <v>577</v>
       </c>
-      <c r="D3" s="86" t="s">
+      <c r="D3" s="88" t="s">
         <v>579</v>
       </c>
-      <c r="E3" s="86" t="s">
+      <c r="E3" s="88" t="s">
         <v>292</v>
       </c>
-      <c r="F3" s="86" t="s">
+      <c r="F3" s="88" t="s">
         <v>578</v>
       </c>
-      <c r="G3" s="68"/>
-      <c r="H3" s="68" t="s">
+      <c r="G3" s="80"/>
+      <c r="H3" s="80" t="s">
         <v>580</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="12.75">
-      <c r="A4" s="69"/>
-      <c r="B4" s="69"/>
-      <c r="C4" s="69"/>
-      <c r="D4" s="69"/>
-      <c r="E4" s="69"/>
-      <c r="F4" s="69"/>
-      <c r="G4" s="69"/>
-      <c r="H4" s="69"/>
+      <c r="A4" s="77"/>
+      <c r="B4" s="77"/>
+      <c r="C4" s="77"/>
+      <c r="D4" s="77"/>
+      <c r="E4" s="77"/>
+      <c r="F4" s="77"/>
+      <c r="G4" s="77"/>
+      <c r="H4" s="77"/>
     </row>
     <row r="5" spans="1:8" ht="15.75" customHeight="1">
       <c r="A5" s="46">
@@ -41143,7 +41138,7 @@
         <v>577</v>
       </c>
       <c r="D9" s="43" t="s">
-        <v>575</v>
+        <v>568</v>
       </c>
       <c r="E9" s="43" t="s">
         <v>292</v>
@@ -41155,7 +41150,7 @@
         <v>589</v>
       </c>
       <c r="H9" s="44" t="s">
-        <v>586</v>
+        <v>692</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.75" customHeight="1">
@@ -41190,9 +41185,7 @@
       <c r="C11" s="43"/>
       <c r="D11" s="43"/>
       <c r="E11" s="43"/>
-      <c r="F11" s="43" t="s">
-        <v>581</v>
-      </c>
+      <c r="F11" s="43"/>
       <c r="G11" s="13"/>
       <c r="H11" s="44"/>
     </row>
@@ -41374,7 +41367,7 @@
       <c r="G19" s="13"/>
       <c r="H19" s="44"/>
     </row>
-    <row r="20" spans="1:8" ht="15.75" customHeight="1">
+    <row r="20" spans="1:8" ht="27" customHeight="1">
       <c r="A20" s="46" t="s">
         <v>598</v>
       </c>
@@ -41416,13 +41409,11 @@
         <v>581</v>
       </c>
       <c r="G21" s="13"/>
-      <c r="H21" s="13" t="s">
-        <v>600</v>
-      </c>
+      <c r="H21" s="13"/>
     </row>
     <row r="22" spans="1:8" ht="15.75" customHeight="1">
       <c r="A22" s="46" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="B22" s="47" t="s">
         <v>485</v>
@@ -41441,7 +41432,7 @@
       </c>
       <c r="G22" s="13"/>
       <c r="H22" s="13" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="15.75" customHeight="1">
@@ -41454,15 +41445,13 @@
       <c r="C23" s="43"/>
       <c r="D23" s="43"/>
       <c r="E23" s="43"/>
-      <c r="F23" s="43" t="s">
-        <v>603</v>
-      </c>
+      <c r="F23" s="43"/>
       <c r="G23" s="13"/>
       <c r="H23" s="44"/>
     </row>
     <row r="24" spans="1:8" ht="15.75" customHeight="1">
       <c r="A24" s="46" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="B24" s="47" t="s">
         <v>495</v>
@@ -41484,12 +41473,14 @@
     </row>
     <row r="25" spans="1:8" ht="15.75" customHeight="1">
       <c r="A25" s="46">
-        <v>44798</v>
+        <v>44812</v>
       </c>
       <c r="B25" s="43" t="s">
         <v>499</v>
       </c>
-      <c r="C25" s="43"/>
+      <c r="C25" s="48" t="s">
+        <v>577</v>
+      </c>
       <c r="D25" s="43" t="s">
         <v>568</v>
       </c>
@@ -41497,19 +41488,21 @@
         <v>292</v>
       </c>
       <c r="F25" s="43" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="G25" s="13"/>
       <c r="H25" s="44"/>
     </row>
     <row r="26" spans="1:8" ht="15.75" customHeight="1">
       <c r="A26" s="46">
-        <v>44798</v>
+        <v>44812</v>
       </c>
       <c r="B26" s="43" t="s">
         <v>504</v>
       </c>
-      <c r="C26" s="43"/>
+      <c r="C26" s="48" t="s">
+        <v>577</v>
+      </c>
       <c r="D26" s="43" t="s">
         <v>568</v>
       </c>
@@ -41517,19 +41510,21 @@
         <v>292</v>
       </c>
       <c r="F26" s="43" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="G26" s="13"/>
       <c r="H26" s="44"/>
     </row>
     <row r="27" spans="1:8" ht="15.75" customHeight="1">
       <c r="A27" s="46">
-        <v>44798</v>
+        <v>44812</v>
       </c>
       <c r="B27" s="43" t="s">
         <v>507</v>
       </c>
-      <c r="C27" s="43"/>
+      <c r="C27" s="48" t="s">
+        <v>577</v>
+      </c>
       <c r="D27" s="43" t="s">
         <v>568</v>
       </c>
@@ -41537,19 +41532,21 @@
         <v>292</v>
       </c>
       <c r="F27" s="43" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="G27" s="13"/>
       <c r="H27" s="44"/>
     </row>
     <row r="28" spans="1:8" ht="15.75" customHeight="1">
       <c r="A28" s="46">
-        <v>44798</v>
+        <v>44812</v>
       </c>
       <c r="B28" s="43" t="s">
         <v>512</v>
       </c>
-      <c r="C28" s="43"/>
+      <c r="C28" s="48" t="s">
+        <v>577</v>
+      </c>
       <c r="D28" s="43" t="s">
         <v>568</v>
       </c>
@@ -41557,19 +41554,21 @@
         <v>292</v>
       </c>
       <c r="F28" s="43" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="G28" s="13"/>
       <c r="H28" s="44"/>
     </row>
     <row r="29" spans="1:8" ht="15.75" customHeight="1">
       <c r="A29" s="46">
-        <v>44798</v>
+        <v>44812</v>
       </c>
       <c r="B29" s="43" t="s">
         <v>516</v>
       </c>
-      <c r="C29" s="43"/>
+      <c r="C29" s="48" t="s">
+        <v>577</v>
+      </c>
       <c r="D29" s="43" t="s">
         <v>568</v>
       </c>
@@ -41577,19 +41576,21 @@
         <v>292</v>
       </c>
       <c r="F29" s="43" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="G29" s="13"/>
       <c r="H29" s="44"/>
     </row>
     <row r="30" spans="1:8" ht="15.75" customHeight="1">
       <c r="A30" s="46">
-        <v>44798</v>
+        <v>44812</v>
       </c>
       <c r="B30" s="43" t="s">
         <v>519</v>
       </c>
-      <c r="C30" s="43"/>
+      <c r="C30" s="48" t="s">
+        <v>577</v>
+      </c>
       <c r="D30" s="43" t="s">
         <v>568</v>
       </c>
@@ -41597,19 +41598,21 @@
         <v>292</v>
       </c>
       <c r="F30" s="43" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="G30" s="13"/>
       <c r="H30" s="44"/>
     </row>
     <row r="31" spans="1:8" ht="15.75" customHeight="1">
       <c r="A31" s="46">
-        <v>44798</v>
+        <v>44812</v>
       </c>
       <c r="B31" s="43" t="s">
         <v>523</v>
       </c>
-      <c r="C31" s="43"/>
+      <c r="C31" s="48" t="s">
+        <v>577</v>
+      </c>
       <c r="D31" s="43" t="s">
         <v>568</v>
       </c>
@@ -41617,19 +41620,21 @@
         <v>292</v>
       </c>
       <c r="F31" s="43" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="G31" s="13"/>
       <c r="H31" s="44"/>
     </row>
     <row r="32" spans="1:8" ht="15.75" customHeight="1">
       <c r="A32" s="46">
-        <v>44798</v>
+        <v>44812</v>
       </c>
       <c r="B32" s="43" t="s">
         <v>524</v>
       </c>
-      <c r="C32" s="43"/>
+      <c r="C32" s="48" t="s">
+        <v>577</v>
+      </c>
       <c r="D32" s="43" t="s">
         <v>568</v>
       </c>
@@ -41637,19 +41642,21 @@
         <v>292</v>
       </c>
       <c r="F32" s="43" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="G32" s="13"/>
       <c r="H32" s="44"/>
     </row>
     <row r="33" spans="1:8" ht="15.75" customHeight="1">
       <c r="A33" s="46">
-        <v>44798</v>
+        <v>44812</v>
       </c>
       <c r="B33" s="43" t="s">
         <v>525</v>
       </c>
-      <c r="C33" s="43"/>
+      <c r="C33" s="48" t="s">
+        <v>577</v>
+      </c>
       <c r="D33" s="43" t="s">
         <v>568</v>
       </c>
@@ -41657,19 +41664,21 @@
         <v>292</v>
       </c>
       <c r="F33" s="43" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="G33" s="13"/>
       <c r="H33" s="44"/>
     </row>
     <row r="34" spans="1:8" ht="15.75" customHeight="1">
       <c r="A34" s="46">
-        <v>44798</v>
+        <v>44812</v>
       </c>
       <c r="B34" s="43" t="s">
         <v>528</v>
       </c>
-      <c r="C34" s="43"/>
+      <c r="C34" s="48" t="s">
+        <v>577</v>
+      </c>
       <c r="D34" s="43" t="s">
         <v>568</v>
       </c>
@@ -41677,17 +41686,21 @@
         <v>292</v>
       </c>
       <c r="F34" s="43" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="G34" s="13"/>
       <c r="H34" s="44"/>
     </row>
     <row r="35" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A35" s="46"/>
+      <c r="A35" s="46">
+        <v>44812</v>
+      </c>
       <c r="B35" s="43" t="s">
         <v>530</v>
       </c>
-      <c r="C35" s="43"/>
+      <c r="C35" s="48" t="s">
+        <v>577</v>
+      </c>
       <c r="D35" s="43" t="s">
         <v>568</v>
       </c>
@@ -41695,7 +41708,7 @@
         <v>292</v>
       </c>
       <c r="F35" s="48" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="G35" s="44"/>
       <c r="H35" s="44"/>
@@ -41724,9 +41737,7 @@
     </row>
     <row r="37" spans="1:8" ht="15.75" customHeight="1">
       <c r="A37" s="46"/>
-      <c r="B37" s="43" t="s">
-        <v>542</v>
-      </c>
+      <c r="B37" s="43"/>
       <c r="C37" s="43"/>
       <c r="D37" s="43"/>
       <c r="E37" s="43"/>
@@ -41736,9 +41747,7 @@
     </row>
     <row r="38" spans="1:8" ht="15.75" customHeight="1">
       <c r="A38" s="46"/>
-      <c r="B38" s="43" t="s">
-        <v>548</v>
-      </c>
+      <c r="B38" s="43"/>
       <c r="C38" s="43"/>
       <c r="D38" s="43"/>
       <c r="E38" s="43"/>
@@ -51393,777 +51402,779 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J15" sqref="J15:J17"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="7.59765625" customWidth="1"/>
-    <col min="2" max="2" width="10.1328125" customWidth="1"/>
-    <col min="3" max="3" width="16.86328125" customWidth="1"/>
+    <col min="1" max="1" width="7.5703125" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" customWidth="1"/>
     <col min="4" max="4" width="26" customWidth="1"/>
-    <col min="5" max="5" width="31.1328125" customWidth="1"/>
-    <col min="6" max="6" width="24.59765625" customWidth="1"/>
-    <col min="7" max="7" width="5.86328125" customWidth="1"/>
-    <col min="8" max="8" width="26.46484375" customWidth="1"/>
-    <col min="9" max="9" width="10.59765625" customWidth="1"/>
+    <col min="5" max="5" width="31.140625" customWidth="1"/>
+    <col min="6" max="6" width="24.5703125" customWidth="1"/>
+    <col min="7" max="7" width="5.85546875" customWidth="1"/>
+    <col min="8" max="8" width="26.42578125" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" customWidth="1"/>
     <col min="10" max="10" width="13" customWidth="1"/>
-    <col min="11" max="14" width="10.59765625" customWidth="1"/>
-    <col min="15" max="15" width="23.59765625" customWidth="1"/>
-    <col min="16" max="26" width="10.59765625" customWidth="1"/>
+    <col min="11" max="14" width="10.5703125" customWidth="1"/>
+    <col min="15" max="15" width="23.5703125" customWidth="1"/>
+    <col min="16" max="26" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="12.75" customHeight="1">
-      <c r="A1" s="101" t="s">
+      <c r="A1" s="102" t="s">
         <v>554</v>
       </c>
-      <c r="B1" s="103" t="s">
+      <c r="B1" s="104" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="103" t="s">
+      <c r="C1" s="104" t="s">
+        <v>605</v>
+      </c>
+      <c r="D1" s="104" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="105" t="s">
         <v>606</v>
       </c>
-      <c r="D1" s="103" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="104" t="s">
+      <c r="F1" s="105" t="s">
         <v>607</v>
       </c>
-      <c r="F1" s="104" t="s">
+      <c r="G1" s="106" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="72"/>
+      <c r="I1" s="101" t="s">
         <v>608</v>
       </c>
-      <c r="G1" s="105" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="75"/>
-      <c r="I1" s="100" t="s">
+      <c r="J1" s="101" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="101" t="s">
         <v>609</v>
       </c>
-      <c r="J1" s="100" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" s="100" t="s">
+      <c r="L1" s="101" t="s">
         <v>610</v>
       </c>
-      <c r="L1" s="100" t="s">
+      <c r="M1" s="101" t="s">
         <v>611</v>
       </c>
-      <c r="M1" s="100" t="s">
+      <c r="N1" s="101" t="s">
         <v>612</v>
       </c>
-      <c r="N1" s="100" t="s">
+      <c r="O1" s="101" t="s">
         <v>613</v>
       </c>
-      <c r="O1" s="100" t="s">
-        <v>614</v>
-      </c>
     </row>
     <row r="2" spans="1:15" ht="12.75" customHeight="1">
-      <c r="A2" s="102"/>
-      <c r="B2" s="69"/>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
-      <c r="F2" s="69"/>
+      <c r="A2" s="103"/>
+      <c r="B2" s="77"/>
+      <c r="C2" s="77"/>
+      <c r="D2" s="77"/>
+      <c r="E2" s="77"/>
+      <c r="F2" s="77"/>
       <c r="G2" s="52" t="s">
         <v>10</v>
       </c>
       <c r="H2" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="69"/>
-      <c r="J2" s="69"/>
-      <c r="K2" s="69"/>
-      <c r="L2" s="69"/>
-      <c r="M2" s="69"/>
-      <c r="N2" s="69"/>
-      <c r="O2" s="69"/>
+      <c r="I2" s="77"/>
+      <c r="J2" s="77"/>
+      <c r="K2" s="77"/>
+      <c r="L2" s="77"/>
+      <c r="M2" s="77"/>
+      <c r="N2" s="77"/>
+      <c r="O2" s="77"/>
     </row>
     <row r="3" spans="1:15" ht="44.25" customHeight="1">
-      <c r="A3" s="91" t="s">
+      <c r="A3" s="98" t="s">
+        <v>614</v>
+      </c>
+      <c r="B3" s="99">
+        <v>44798</v>
+      </c>
+      <c r="C3" s="100" t="s">
         <v>615</v>
       </c>
-      <c r="B3" s="107">
-        <v>44798</v>
-      </c>
-      <c r="C3" s="89" t="s">
+      <c r="D3" s="81" t="s">
         <v>616</v>
       </c>
-      <c r="D3" s="70" t="s">
+      <c r="E3" s="81" t="s">
         <v>617</v>
       </c>
-      <c r="E3" s="70" t="s">
+      <c r="F3" s="81" t="s">
         <v>618</v>
-      </c>
-      <c r="F3" s="70" t="s">
-        <v>619</v>
       </c>
       <c r="G3" s="53">
         <v>1</v>
       </c>
       <c r="H3" s="17" t="s">
+        <v>619</v>
+      </c>
+      <c r="I3" s="81" t="s">
+        <v>292</v>
+      </c>
+      <c r="J3" s="81" t="s">
         <v>620</v>
       </c>
-      <c r="I3" s="70" t="s">
-        <v>292</v>
-      </c>
-      <c r="J3" s="70" t="s">
+      <c r="K3" s="81" t="s">
         <v>621</v>
       </c>
-      <c r="K3" s="70" t="s">
+      <c r="L3" s="81" t="s">
+        <v>621</v>
+      </c>
+      <c r="M3" s="81" t="s">
+        <v>202</v>
+      </c>
+      <c r="N3" s="81" t="s">
         <v>622</v>
       </c>
-      <c r="L3" s="70" t="s">
-        <v>622</v>
-      </c>
-      <c r="M3" s="70" t="s">
-        <v>202</v>
-      </c>
-      <c r="N3" s="70" t="s">
+      <c r="O3" s="96" t="s">
         <v>623</v>
       </c>
-      <c r="O3" s="106" t="s">
+    </row>
+    <row r="4" spans="1:15" ht="12.75" customHeight="1">
+      <c r="A4" s="91"/>
+      <c r="B4" s="91"/>
+      <c r="C4" s="91"/>
+      <c r="D4" s="91"/>
+      <c r="E4" s="91"/>
+      <c r="F4" s="91"/>
+      <c r="G4" s="97">
+        <v>2</v>
+      </c>
+      <c r="H4" s="81" t="s">
         <v>624</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" ht="12.75" customHeight="1">
-      <c r="A4" s="88"/>
-      <c r="B4" s="88"/>
-      <c r="C4" s="88"/>
-      <c r="D4" s="88"/>
-      <c r="E4" s="88"/>
-      <c r="F4" s="88"/>
-      <c r="G4" s="87">
-        <v>2</v>
-      </c>
-      <c r="H4" s="70" t="s">
+      <c r="I4" s="91"/>
+      <c r="J4" s="91"/>
+      <c r="K4" s="91"/>
+      <c r="L4" s="91"/>
+      <c r="M4" s="91"/>
+      <c r="N4" s="91"/>
+      <c r="O4" s="91"/>
+    </row>
+    <row r="5" spans="1:15" ht="12.75" customHeight="1">
+      <c r="A5" s="91"/>
+      <c r="B5" s="91"/>
+      <c r="C5" s="91"/>
+      <c r="D5" s="91"/>
+      <c r="E5" s="91"/>
+      <c r="F5" s="91"/>
+      <c r="G5" s="91"/>
+      <c r="H5" s="91"/>
+      <c r="I5" s="91"/>
+      <c r="J5" s="91"/>
+      <c r="K5" s="91"/>
+      <c r="L5" s="91"/>
+      <c r="M5" s="91"/>
+      <c r="N5" s="91"/>
+      <c r="O5" s="91"/>
+    </row>
+    <row r="6" spans="1:15" ht="12.75" customHeight="1">
+      <c r="A6" s="91"/>
+      <c r="B6" s="91"/>
+      <c r="C6" s="91"/>
+      <c r="D6" s="91"/>
+      <c r="E6" s="91"/>
+      <c r="F6" s="91"/>
+      <c r="G6" s="91"/>
+      <c r="H6" s="91"/>
+      <c r="I6" s="91"/>
+      <c r="J6" s="91"/>
+      <c r="K6" s="91"/>
+      <c r="L6" s="91"/>
+      <c r="M6" s="91"/>
+      <c r="N6" s="91"/>
+      <c r="O6" s="91"/>
+    </row>
+    <row r="7" spans="1:15" ht="20.25" customHeight="1">
+      <c r="A7" s="77"/>
+      <c r="B7" s="77"/>
+      <c r="C7" s="77"/>
+      <c r="D7" s="77"/>
+      <c r="E7" s="77"/>
+      <c r="F7" s="77"/>
+      <c r="G7" s="77"/>
+      <c r="H7" s="77"/>
+      <c r="I7" s="77"/>
+      <c r="J7" s="77"/>
+      <c r="K7" s="77"/>
+      <c r="L7" s="77"/>
+      <c r="M7" s="77"/>
+      <c r="N7" s="77"/>
+      <c r="O7" s="77"/>
+    </row>
+    <row r="8" spans="1:15" ht="34.5" customHeight="1">
+      <c r="A8" s="100" t="s">
         <v>625</v>
       </c>
-      <c r="I4" s="88"/>
-      <c r="J4" s="88"/>
-      <c r="K4" s="88"/>
-      <c r="L4" s="88"/>
-      <c r="M4" s="88"/>
-      <c r="N4" s="88"/>
-      <c r="O4" s="88"/>
-    </row>
-    <row r="5" spans="1:15" ht="12.75" customHeight="1">
-      <c r="A5" s="88"/>
-      <c r="B5" s="88"/>
-      <c r="C5" s="88"/>
-      <c r="D5" s="88"/>
-      <c r="E5" s="88"/>
-      <c r="F5" s="88"/>
-      <c r="G5" s="88"/>
-      <c r="H5" s="88"/>
-      <c r="I5" s="88"/>
-      <c r="J5" s="88"/>
-      <c r="K5" s="88"/>
-      <c r="L5" s="88"/>
-      <c r="M5" s="88"/>
-      <c r="N5" s="88"/>
-      <c r="O5" s="88"/>
-    </row>
-    <row r="6" spans="1:15" ht="12.75" customHeight="1">
-      <c r="A6" s="88"/>
-      <c r="B6" s="88"/>
-      <c r="C6" s="88"/>
-      <c r="D6" s="88"/>
-      <c r="E6" s="88"/>
-      <c r="F6" s="88"/>
-      <c r="G6" s="88"/>
-      <c r="H6" s="88"/>
-      <c r="I6" s="88"/>
-      <c r="J6" s="88"/>
-      <c r="K6" s="88"/>
-      <c r="L6" s="88"/>
-      <c r="M6" s="88"/>
-      <c r="N6" s="88"/>
-      <c r="O6" s="88"/>
-    </row>
-    <row r="7" spans="1:15" ht="20.25" customHeight="1">
-      <c r="A7" s="69"/>
-      <c r="B7" s="69"/>
-      <c r="C7" s="69"/>
-      <c r="D7" s="69"/>
-      <c r="E7" s="69"/>
-      <c r="F7" s="69"/>
-      <c r="G7" s="69"/>
-      <c r="H7" s="69"/>
-      <c r="I7" s="69"/>
-      <c r="J7" s="69"/>
-      <c r="K7" s="69"/>
-      <c r="L7" s="69"/>
-      <c r="M7" s="69"/>
-      <c r="N7" s="69"/>
-      <c r="O7" s="69"/>
-    </row>
-    <row r="8" spans="1:15" ht="34.5" customHeight="1">
-      <c r="A8" s="89" t="s">
+      <c r="B8" s="110">
+        <v>44798</v>
+      </c>
+      <c r="C8" s="100" t="s">
         <v>626</v>
       </c>
-      <c r="B8" s="90">
-        <v>44798</v>
-      </c>
-      <c r="C8" s="89" t="s">
+      <c r="D8" s="81" t="s">
         <v>627</v>
       </c>
-      <c r="D8" s="70" t="s">
+      <c r="E8" s="81" t="s">
         <v>628</v>
       </c>
-      <c r="E8" s="70" t="s">
+      <c r="F8" s="81" t="s">
         <v>629</v>
-      </c>
-      <c r="F8" s="70" t="s">
-        <v>630</v>
       </c>
       <c r="G8" s="53">
         <v>1</v>
       </c>
       <c r="H8" s="17" t="s">
+        <v>619</v>
+      </c>
+      <c r="I8" s="81" t="s">
+        <v>292</v>
+      </c>
+      <c r="J8" s="81" t="s">
         <v>620</v>
       </c>
-      <c r="I8" s="70" t="s">
-        <v>292</v>
-      </c>
-      <c r="J8" s="70" t="s">
+      <c r="K8" s="81" t="s">
         <v>621</v>
       </c>
-      <c r="K8" s="70" t="s">
-        <v>622</v>
-      </c>
-      <c r="L8" s="70" t="s">
-        <v>622</v>
-      </c>
-      <c r="M8" s="70" t="s">
+      <c r="L8" s="81" t="s">
+        <v>621</v>
+      </c>
+      <c r="M8" s="81" t="s">
         <v>202</v>
       </c>
-      <c r="N8" s="70" t="s">
+      <c r="N8" s="81" t="s">
+        <v>630</v>
+      </c>
+      <c r="O8" s="96" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="12.75" customHeight="1">
+      <c r="A9" s="91"/>
+      <c r="B9" s="91"/>
+      <c r="C9" s="91"/>
+      <c r="D9" s="91"/>
+      <c r="E9" s="91"/>
+      <c r="F9" s="91"/>
+      <c r="G9" s="97">
+        <v>2</v>
+      </c>
+      <c r="H9" s="81" t="s">
+        <v>624</v>
+      </c>
+      <c r="I9" s="91"/>
+      <c r="J9" s="91"/>
+      <c r="K9" s="91"/>
+      <c r="L9" s="91"/>
+      <c r="M9" s="91"/>
+      <c r="N9" s="91"/>
+      <c r="O9" s="91"/>
+    </row>
+    <row r="10" spans="1:15" ht="12.75" customHeight="1">
+      <c r="A10" s="91"/>
+      <c r="B10" s="91"/>
+      <c r="C10" s="91"/>
+      <c r="D10" s="91"/>
+      <c r="E10" s="91"/>
+      <c r="F10" s="91"/>
+      <c r="G10" s="91"/>
+      <c r="H10" s="91"/>
+      <c r="I10" s="91"/>
+      <c r="J10" s="91"/>
+      <c r="K10" s="91"/>
+      <c r="L10" s="91"/>
+      <c r="M10" s="91"/>
+      <c r="N10" s="91"/>
+      <c r="O10" s="91"/>
+    </row>
+    <row r="11" spans="1:15" ht="12.75" customHeight="1">
+      <c r="A11" s="77"/>
+      <c r="B11" s="77"/>
+      <c r="C11" s="77"/>
+      <c r="D11" s="77"/>
+      <c r="E11" s="77"/>
+      <c r="F11" s="77"/>
+      <c r="G11" s="77"/>
+      <c r="H11" s="77"/>
+      <c r="I11" s="77"/>
+      <c r="J11" s="77"/>
+      <c r="K11" s="77"/>
+      <c r="L11" s="77"/>
+      <c r="M11" s="77"/>
+      <c r="N11" s="77"/>
+      <c r="O11" s="77"/>
+    </row>
+    <row r="12" spans="1:15" ht="12.75" customHeight="1">
+      <c r="A12" s="98" t="s">
+        <v>585</v>
+      </c>
+      <c r="B12" s="109">
+        <v>44811</v>
+      </c>
+      <c r="C12" s="100" t="s">
         <v>631</v>
       </c>
-      <c r="O8" s="106" t="s">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" ht="12.75" customHeight="1">
-      <c r="A9" s="88"/>
-      <c r="B9" s="88"/>
-      <c r="C9" s="88"/>
-      <c r="D9" s="88"/>
-      <c r="E9" s="88"/>
-      <c r="F9" s="88"/>
-      <c r="G9" s="87">
-        <v>2</v>
-      </c>
-      <c r="H9" s="70" t="s">
-        <v>625</v>
-      </c>
-      <c r="I9" s="88"/>
-      <c r="J9" s="88"/>
-      <c r="K9" s="88"/>
-      <c r="L9" s="88"/>
-      <c r="M9" s="88"/>
-      <c r="N9" s="88"/>
-      <c r="O9" s="88"/>
-    </row>
-    <row r="10" spans="1:15" ht="12.75" customHeight="1">
-      <c r="A10" s="88"/>
-      <c r="B10" s="88"/>
-      <c r="C10" s="88"/>
-      <c r="D10" s="88"/>
-      <c r="E10" s="88"/>
-      <c r="F10" s="88"/>
-      <c r="G10" s="88"/>
-      <c r="H10" s="88"/>
-      <c r="I10" s="88"/>
-      <c r="J10" s="88"/>
-      <c r="K10" s="88"/>
-      <c r="L10" s="88"/>
-      <c r="M10" s="88"/>
-      <c r="N10" s="88"/>
-      <c r="O10" s="88"/>
-    </row>
-    <row r="11" spans="1:15" ht="12.75" customHeight="1">
-      <c r="A11" s="69"/>
-      <c r="B11" s="69"/>
-      <c r="C11" s="69"/>
-      <c r="D11" s="69"/>
-      <c r="E11" s="69"/>
-      <c r="F11" s="69"/>
-      <c r="G11" s="69"/>
-      <c r="H11" s="69"/>
-      <c r="I11" s="69"/>
-      <c r="J11" s="69"/>
-      <c r="K11" s="69"/>
-      <c r="L11" s="69"/>
-      <c r="M11" s="69"/>
-      <c r="N11" s="69"/>
-      <c r="O11" s="69"/>
-    </row>
-    <row r="12" spans="1:15" ht="12.75" customHeight="1">
-      <c r="A12" s="91" t="s">
-        <v>585</v>
-      </c>
-      <c r="B12" s="92">
-        <v>44811</v>
-      </c>
-      <c r="C12" s="89" t="s">
+      <c r="D12" s="81" t="s">
         <v>632</v>
       </c>
-      <c r="D12" s="70" t="s">
+      <c r="E12" s="81" t="s">
         <v>633</v>
       </c>
-      <c r="E12" s="70" t="s">
+      <c r="F12" s="81" t="s">
         <v>634</v>
-      </c>
-      <c r="F12" s="70" t="s">
-        <v>635</v>
       </c>
       <c r="G12" s="17">
         <v>1</v>
       </c>
       <c r="H12" s="17" t="s">
+        <v>635</v>
+      </c>
+      <c r="I12" s="81" t="s">
+        <v>292</v>
+      </c>
+      <c r="J12" s="88" t="s">
+        <v>620</v>
+      </c>
+      <c r="K12" s="81" t="s">
         <v>636</v>
       </c>
-      <c r="I12" s="70" t="s">
-        <v>292</v>
-      </c>
-      <c r="J12" s="86" t="s">
+      <c r="L12" s="81" t="s">
         <v>637</v>
       </c>
-      <c r="K12" s="70" t="s">
+      <c r="M12" s="81" t="s">
+        <v>133</v>
+      </c>
+      <c r="N12" s="81" t="s">
         <v>638</v>
       </c>
-      <c r="L12" s="70" t="s">
-        <v>639</v>
-      </c>
-      <c r="M12" s="70" t="s">
-        <v>133</v>
-      </c>
-      <c r="N12" s="70" t="s">
-        <v>640</v>
-      </c>
-      <c r="O12" s="70"/>
+      <c r="O12" s="81"/>
     </row>
     <row r="13" spans="1:15" ht="12.75" customHeight="1">
-      <c r="A13" s="88"/>
-      <c r="B13" s="88"/>
-      <c r="C13" s="88"/>
-      <c r="D13" s="88"/>
-      <c r="E13" s="88"/>
-      <c r="F13" s="88"/>
+      <c r="A13" s="91"/>
+      <c r="B13" s="91"/>
+      <c r="C13" s="91"/>
+      <c r="D13" s="91"/>
+      <c r="E13" s="91"/>
+      <c r="F13" s="91"/>
       <c r="G13" s="17">
         <v>2</v>
       </c>
       <c r="H13" s="17" t="s">
-        <v>641</v>
-      </c>
-      <c r="I13" s="88"/>
-      <c r="J13" s="88"/>
-      <c r="K13" s="88"/>
-      <c r="L13" s="88"/>
-      <c r="M13" s="88"/>
-      <c r="N13" s="88"/>
-      <c r="O13" s="88"/>
+        <v>639</v>
+      </c>
+      <c r="I13" s="91"/>
+      <c r="J13" s="91"/>
+      <c r="K13" s="91"/>
+      <c r="L13" s="91"/>
+      <c r="M13" s="91"/>
+      <c r="N13" s="91"/>
+      <c r="O13" s="91"/>
     </row>
     <row r="14" spans="1:15" ht="27.75" customHeight="1">
-      <c r="A14" s="69"/>
-      <c r="B14" s="69"/>
-      <c r="C14" s="69"/>
-      <c r="D14" s="69"/>
-      <c r="E14" s="69"/>
-      <c r="F14" s="69"/>
+      <c r="A14" s="77"/>
+      <c r="B14" s="77"/>
+      <c r="C14" s="77"/>
+      <c r="D14" s="77"/>
+      <c r="E14" s="77"/>
+      <c r="F14" s="77"/>
       <c r="G14" s="17">
         <v>3</v>
       </c>
       <c r="H14" s="17" t="s">
+        <v>640</v>
+      </c>
+      <c r="I14" s="77"/>
+      <c r="J14" s="77"/>
+      <c r="K14" s="77"/>
+      <c r="L14" s="77"/>
+      <c r="M14" s="77"/>
+      <c r="N14" s="77"/>
+      <c r="O14" s="77"/>
+    </row>
+    <row r="15" spans="1:15" ht="12.75" customHeight="1">
+      <c r="A15" s="98" t="s">
+        <v>589</v>
+      </c>
+      <c r="B15" s="109">
+        <v>44811</v>
+      </c>
+      <c r="C15" s="100" t="s">
+        <v>641</v>
+      </c>
+      <c r="D15" s="81" t="s">
+        <v>632</v>
+      </c>
+      <c r="E15" s="81" t="s">
+        <v>633</v>
+      </c>
+      <c r="F15" s="81" t="s">
         <v>642</v>
-      </c>
-      <c r="I14" s="69"/>
-      <c r="J14" s="69"/>
-      <c r="K14" s="69"/>
-      <c r="L14" s="69"/>
-      <c r="M14" s="69"/>
-      <c r="N14" s="69"/>
-      <c r="O14" s="69"/>
-    </row>
-    <row r="15" spans="1:15" ht="12.75" customHeight="1">
-      <c r="A15" s="91" t="s">
-        <v>589</v>
-      </c>
-      <c r="B15" s="92">
-        <v>44811</v>
-      </c>
-      <c r="C15" s="89" t="s">
-        <v>643</v>
-      </c>
-      <c r="D15" s="70" t="s">
-        <v>633</v>
-      </c>
-      <c r="E15" s="70" t="s">
-        <v>634</v>
-      </c>
-      <c r="F15" s="70" t="s">
-        <v>644</v>
       </c>
       <c r="G15" s="17">
         <v>4</v>
       </c>
       <c r="H15" s="17" t="s">
+        <v>635</v>
+      </c>
+      <c r="I15" s="81" t="s">
+        <v>292</v>
+      </c>
+      <c r="J15" s="88" t="s">
+        <v>620</v>
+      </c>
+      <c r="K15" s="81" t="s">
         <v>636</v>
       </c>
-      <c r="I15" s="70" t="s">
-        <v>292</v>
-      </c>
-      <c r="J15" s="86" t="s">
+      <c r="L15" s="81" t="s">
         <v>637</v>
       </c>
-      <c r="K15" s="70" t="s">
+      <c r="M15" s="81" t="s">
+        <v>133</v>
+      </c>
+      <c r="N15" s="81" t="s">
         <v>638</v>
       </c>
-      <c r="L15" s="70" t="s">
-        <v>639</v>
-      </c>
-      <c r="M15" s="70" t="s">
-        <v>133</v>
-      </c>
-      <c r="N15" s="70" t="s">
-        <v>640</v>
-      </c>
-      <c r="O15" s="70"/>
+      <c r="O15" s="81"/>
     </row>
     <row r="16" spans="1:15" ht="29.25" customHeight="1">
-      <c r="A16" s="88"/>
-      <c r="B16" s="88"/>
-      <c r="C16" s="88"/>
-      <c r="D16" s="88"/>
-      <c r="E16" s="88"/>
-      <c r="F16" s="88"/>
+      <c r="A16" s="91"/>
+      <c r="B16" s="91"/>
+      <c r="C16" s="91"/>
+      <c r="D16" s="91"/>
+      <c r="E16" s="91"/>
+      <c r="F16" s="91"/>
       <c r="G16" s="17">
         <v>5</v>
       </c>
       <c r="H16" s="17" t="s">
-        <v>641</v>
-      </c>
-      <c r="I16" s="88"/>
-      <c r="J16" s="88"/>
-      <c r="K16" s="88"/>
-      <c r="L16" s="88"/>
-      <c r="M16" s="88"/>
-      <c r="N16" s="88"/>
-      <c r="O16" s="88"/>
+        <v>639</v>
+      </c>
+      <c r="I16" s="91"/>
+      <c r="J16" s="91"/>
+      <c r="K16" s="91"/>
+      <c r="L16" s="91"/>
+      <c r="M16" s="91"/>
+      <c r="N16" s="91"/>
+      <c r="O16" s="91"/>
     </row>
     <row r="17" spans="1:15" ht="45" customHeight="1">
-      <c r="A17" s="69"/>
-      <c r="B17" s="69"/>
-      <c r="C17" s="69"/>
-      <c r="D17" s="69"/>
-      <c r="E17" s="69"/>
-      <c r="F17" s="69"/>
+      <c r="A17" s="77"/>
+      <c r="B17" s="77"/>
+      <c r="C17" s="77"/>
+      <c r="D17" s="77"/>
+      <c r="E17" s="77"/>
+      <c r="F17" s="77"/>
       <c r="G17" s="17">
         <v>6</v>
       </c>
       <c r="H17" s="17" t="s">
-        <v>642</v>
-      </c>
-      <c r="I17" s="69"/>
-      <c r="J17" s="69"/>
-      <c r="K17" s="69"/>
-      <c r="L17" s="69"/>
-      <c r="M17" s="69"/>
-      <c r="N17" s="69"/>
-      <c r="O17" s="69"/>
+        <v>640</v>
+      </c>
+      <c r="I17" s="77"/>
+      <c r="J17" s="77"/>
+      <c r="K17" s="77"/>
+      <c r="L17" s="77"/>
+      <c r="M17" s="77"/>
+      <c r="N17" s="77"/>
+      <c r="O17" s="77"/>
     </row>
     <row r="18" spans="1:15" ht="12.75" customHeight="1">
-      <c r="A18" s="93"/>
-      <c r="B18" s="94"/>
-      <c r="C18" s="95"/>
-      <c r="D18" s="96"/>
-      <c r="E18" s="70"/>
-      <c r="F18" s="70"/>
+      <c r="A18" s="90"/>
+      <c r="B18" s="92"/>
+      <c r="C18" s="93"/>
+      <c r="D18" s="108"/>
+      <c r="E18" s="81"/>
+      <c r="F18" s="81"/>
       <c r="G18" s="17"/>
       <c r="H18" s="17"/>
-      <c r="I18" s="97"/>
-      <c r="J18" s="86"/>
-      <c r="K18" s="70"/>
-      <c r="L18" s="70"/>
-      <c r="M18" s="86"/>
-      <c r="N18" s="70"/>
-      <c r="O18" s="70"/>
+      <c r="I18" s="107"/>
+      <c r="J18" s="88"/>
+      <c r="K18" s="81"/>
+      <c r="L18" s="81"/>
+      <c r="M18" s="88"/>
+      <c r="N18" s="81"/>
+      <c r="O18" s="81"/>
     </row>
     <row r="19" spans="1:15" ht="12.75" customHeight="1">
-      <c r="A19" s="88"/>
-      <c r="B19" s="88"/>
-      <c r="C19" s="88"/>
-      <c r="D19" s="88"/>
-      <c r="E19" s="88"/>
-      <c r="F19" s="88"/>
+      <c r="A19" s="91"/>
+      <c r="B19" s="91"/>
+      <c r="C19" s="91"/>
+      <c r="D19" s="91"/>
+      <c r="E19" s="91"/>
+      <c r="F19" s="91"/>
       <c r="G19" s="17"/>
       <c r="H19" s="17"/>
-      <c r="I19" s="88"/>
-      <c r="J19" s="88"/>
-      <c r="K19" s="88"/>
-      <c r="L19" s="88"/>
-      <c r="M19" s="88"/>
-      <c r="N19" s="88"/>
-      <c r="O19" s="88"/>
+      <c r="I19" s="91"/>
+      <c r="J19" s="91"/>
+      <c r="K19" s="91"/>
+      <c r="L19" s="91"/>
+      <c r="M19" s="91"/>
+      <c r="N19" s="91"/>
+      <c r="O19" s="91"/>
     </row>
     <row r="20" spans="1:15" ht="12.75" customHeight="1">
-      <c r="A20" s="88"/>
-      <c r="B20" s="88"/>
-      <c r="C20" s="88"/>
-      <c r="D20" s="88"/>
-      <c r="E20" s="88"/>
-      <c r="F20" s="88"/>
+      <c r="A20" s="91"/>
+      <c r="B20" s="91"/>
+      <c r="C20" s="91"/>
+      <c r="D20" s="91"/>
+      <c r="E20" s="91"/>
+      <c r="F20" s="91"/>
       <c r="G20" s="17"/>
       <c r="H20" s="17"/>
-      <c r="I20" s="88"/>
-      <c r="J20" s="88"/>
-      <c r="K20" s="88"/>
-      <c r="L20" s="88"/>
-      <c r="M20" s="88"/>
-      <c r="N20" s="88"/>
-      <c r="O20" s="88"/>
+      <c r="I20" s="91"/>
+      <c r="J20" s="91"/>
+      <c r="K20" s="91"/>
+      <c r="L20" s="91"/>
+      <c r="M20" s="91"/>
+      <c r="N20" s="91"/>
+      <c r="O20" s="91"/>
     </row>
     <row r="21" spans="1:15" ht="12.75" customHeight="1">
-      <c r="A21" s="69"/>
-      <c r="B21" s="69"/>
-      <c r="C21" s="69"/>
-      <c r="D21" s="69"/>
-      <c r="E21" s="69"/>
-      <c r="F21" s="69"/>
+      <c r="A21" s="77"/>
+      <c r="B21" s="77"/>
+      <c r="C21" s="77"/>
+      <c r="D21" s="77"/>
+      <c r="E21" s="77"/>
+      <c r="F21" s="77"/>
       <c r="G21" s="17"/>
       <c r="H21" s="17"/>
-      <c r="I21" s="69"/>
-      <c r="J21" s="69"/>
-      <c r="K21" s="69"/>
-      <c r="L21" s="69"/>
-      <c r="M21" s="69"/>
-      <c r="N21" s="69"/>
-      <c r="O21" s="69"/>
+      <c r="I21" s="77"/>
+      <c r="J21" s="77"/>
+      <c r="K21" s="77"/>
+      <c r="L21" s="77"/>
+      <c r="M21" s="77"/>
+      <c r="N21" s="77"/>
+      <c r="O21" s="77"/>
     </row>
     <row r="22" spans="1:15" ht="12.75" customHeight="1">
-      <c r="A22" s="93"/>
-      <c r="B22" s="94"/>
-      <c r="C22" s="95"/>
-      <c r="D22" s="96"/>
-      <c r="E22" s="98"/>
-      <c r="F22" s="98"/>
+      <c r="A22" s="90"/>
+      <c r="B22" s="92"/>
+      <c r="C22" s="93"/>
+      <c r="D22" s="108"/>
+      <c r="E22" s="95"/>
+      <c r="F22" s="95"/>
       <c r="G22" s="17"/>
       <c r="H22" s="17"/>
-      <c r="I22" s="70"/>
-      <c r="J22" s="86"/>
-      <c r="K22" s="70"/>
-      <c r="L22" s="70"/>
-      <c r="M22" s="70"/>
-      <c r="N22" s="70"/>
-      <c r="O22" s="70"/>
+      <c r="I22" s="81"/>
+      <c r="J22" s="88"/>
+      <c r="K22" s="81"/>
+      <c r="L22" s="81"/>
+      <c r="M22" s="81"/>
+      <c r="N22" s="81"/>
+      <c r="O22" s="81"/>
     </row>
     <row r="23" spans="1:15" ht="12.75" customHeight="1">
-      <c r="A23" s="88"/>
-      <c r="B23" s="88"/>
-      <c r="C23" s="88"/>
-      <c r="D23" s="88"/>
-      <c r="E23" s="88"/>
-      <c r="F23" s="88"/>
+      <c r="A23" s="91"/>
+      <c r="B23" s="91"/>
+      <c r="C23" s="91"/>
+      <c r="D23" s="91"/>
+      <c r="E23" s="91"/>
+      <c r="F23" s="91"/>
       <c r="G23" s="17"/>
       <c r="H23" s="17"/>
-      <c r="I23" s="88"/>
-      <c r="J23" s="88"/>
-      <c r="K23" s="88"/>
-      <c r="L23" s="88"/>
-      <c r="M23" s="88"/>
-      <c r="N23" s="88"/>
-      <c r="O23" s="88"/>
+      <c r="I23" s="91"/>
+      <c r="J23" s="91"/>
+      <c r="K23" s="91"/>
+      <c r="L23" s="91"/>
+      <c r="M23" s="91"/>
+      <c r="N23" s="91"/>
+      <c r="O23" s="91"/>
     </row>
     <row r="24" spans="1:15" ht="12.75" customHeight="1">
-      <c r="A24" s="88"/>
-      <c r="B24" s="88"/>
-      <c r="C24" s="88"/>
-      <c r="D24" s="88"/>
-      <c r="E24" s="88"/>
-      <c r="F24" s="88"/>
+      <c r="A24" s="91"/>
+      <c r="B24" s="91"/>
+      <c r="C24" s="91"/>
+      <c r="D24" s="91"/>
+      <c r="E24" s="91"/>
+      <c r="F24" s="91"/>
       <c r="G24" s="17"/>
       <c r="H24" s="17"/>
-      <c r="I24" s="88"/>
-      <c r="J24" s="88"/>
-      <c r="K24" s="88"/>
-      <c r="L24" s="88"/>
-      <c r="M24" s="88"/>
-      <c r="N24" s="88"/>
-      <c r="O24" s="88"/>
+      <c r="I24" s="91"/>
+      <c r="J24" s="91"/>
+      <c r="K24" s="91"/>
+      <c r="L24" s="91"/>
+      <c r="M24" s="91"/>
+      <c r="N24" s="91"/>
+      <c r="O24" s="91"/>
     </row>
     <row r="25" spans="1:15" ht="12.75" customHeight="1">
-      <c r="A25" s="88"/>
-      <c r="B25" s="88"/>
-      <c r="C25" s="88"/>
-      <c r="D25" s="88"/>
-      <c r="E25" s="88"/>
-      <c r="F25" s="88"/>
+      <c r="A25" s="91"/>
+      <c r="B25" s="91"/>
+      <c r="C25" s="91"/>
+      <c r="D25" s="91"/>
+      <c r="E25" s="91"/>
+      <c r="F25" s="91"/>
       <c r="G25" s="17"/>
       <c r="H25" s="17"/>
-      <c r="I25" s="88"/>
-      <c r="J25" s="88"/>
-      <c r="K25" s="88"/>
-      <c r="L25" s="88"/>
-      <c r="M25" s="88"/>
-      <c r="N25" s="88"/>
-      <c r="O25" s="88"/>
+      <c r="I25" s="91"/>
+      <c r="J25" s="91"/>
+      <c r="K25" s="91"/>
+      <c r="L25" s="91"/>
+      <c r="M25" s="91"/>
+      <c r="N25" s="91"/>
+      <c r="O25" s="91"/>
     </row>
     <row r="26" spans="1:15" ht="12.75" customHeight="1">
-      <c r="A26" s="69"/>
-      <c r="B26" s="69"/>
-      <c r="C26" s="69"/>
-      <c r="D26" s="69"/>
-      <c r="E26" s="69"/>
-      <c r="F26" s="69"/>
+      <c r="A26" s="77"/>
+      <c r="B26" s="77"/>
+      <c r="C26" s="77"/>
+      <c r="D26" s="77"/>
+      <c r="E26" s="77"/>
+      <c r="F26" s="77"/>
       <c r="G26" s="17"/>
       <c r="H26" s="17"/>
-      <c r="I26" s="69"/>
-      <c r="J26" s="69"/>
-      <c r="K26" s="69"/>
-      <c r="L26" s="69"/>
-      <c r="M26" s="69"/>
-      <c r="N26" s="69"/>
-      <c r="O26" s="69"/>
+      <c r="I26" s="77"/>
+      <c r="J26" s="77"/>
+      <c r="K26" s="77"/>
+      <c r="L26" s="77"/>
+      <c r="M26" s="77"/>
+      <c r="N26" s="77"/>
+      <c r="O26" s="77"/>
     </row>
     <row r="27" spans="1:15" ht="12.75" customHeight="1">
-      <c r="A27" s="93"/>
-      <c r="B27" s="94"/>
-      <c r="C27" s="95"/>
-      <c r="D27" s="99"/>
-      <c r="E27" s="98"/>
-      <c r="F27" s="98"/>
+      <c r="A27" s="90"/>
+      <c r="B27" s="92"/>
+      <c r="C27" s="93"/>
+      <c r="D27" s="94"/>
+      <c r="E27" s="95"/>
+      <c r="F27" s="95"/>
       <c r="G27" s="17"/>
       <c r="H27" s="17"/>
-      <c r="I27" s="97"/>
-      <c r="J27" s="86"/>
-      <c r="K27" s="70"/>
-      <c r="L27" s="70"/>
-      <c r="M27" s="86"/>
-      <c r="N27" s="70"/>
-      <c r="O27" s="70"/>
+      <c r="I27" s="107"/>
+      <c r="J27" s="88"/>
+      <c r="K27" s="81"/>
+      <c r="L27" s="81"/>
+      <c r="M27" s="88"/>
+      <c r="N27" s="81"/>
+      <c r="O27" s="81"/>
     </row>
     <row r="28" spans="1:15" ht="12.75" customHeight="1">
-      <c r="A28" s="88"/>
-      <c r="B28" s="88"/>
-      <c r="C28" s="88"/>
-      <c r="D28" s="88"/>
-      <c r="E28" s="88"/>
-      <c r="F28" s="88"/>
+      <c r="A28" s="91"/>
+      <c r="B28" s="91"/>
+      <c r="C28" s="91"/>
+      <c r="D28" s="91"/>
+      <c r="E28" s="91"/>
+      <c r="F28" s="91"/>
       <c r="G28" s="17"/>
       <c r="H28" s="17"/>
-      <c r="I28" s="88"/>
-      <c r="J28" s="88"/>
-      <c r="K28" s="88"/>
-      <c r="L28" s="88"/>
-      <c r="M28" s="88"/>
-      <c r="N28" s="88"/>
-      <c r="O28" s="88"/>
+      <c r="I28" s="91"/>
+      <c r="J28" s="91"/>
+      <c r="K28" s="91"/>
+      <c r="L28" s="91"/>
+      <c r="M28" s="91"/>
+      <c r="N28" s="91"/>
+      <c r="O28" s="91"/>
     </row>
     <row r="29" spans="1:15" ht="12.75" customHeight="1">
-      <c r="A29" s="88"/>
-      <c r="B29" s="88"/>
-      <c r="C29" s="88"/>
-      <c r="D29" s="88"/>
-      <c r="E29" s="88"/>
-      <c r="F29" s="88"/>
+      <c r="A29" s="91"/>
+      <c r="B29" s="91"/>
+      <c r="C29" s="91"/>
+      <c r="D29" s="91"/>
+      <c r="E29" s="91"/>
+      <c r="F29" s="91"/>
       <c r="G29" s="17"/>
       <c r="H29" s="17"/>
-      <c r="I29" s="88"/>
-      <c r="J29" s="88"/>
-      <c r="K29" s="88"/>
-      <c r="L29" s="88"/>
-      <c r="M29" s="88"/>
-      <c r="N29" s="88"/>
-      <c r="O29" s="88"/>
+      <c r="I29" s="91"/>
+      <c r="J29" s="91"/>
+      <c r="K29" s="91"/>
+      <c r="L29" s="91"/>
+      <c r="M29" s="91"/>
+      <c r="N29" s="91"/>
+      <c r="O29" s="91"/>
     </row>
     <row r="30" spans="1:15" ht="12.75" customHeight="1">
-      <c r="A30" s="69"/>
-      <c r="B30" s="69"/>
-      <c r="C30" s="69"/>
-      <c r="D30" s="69"/>
-      <c r="E30" s="69"/>
-      <c r="F30" s="69"/>
+      <c r="A30" s="77"/>
+      <c r="B30" s="77"/>
+      <c r="C30" s="77"/>
+      <c r="D30" s="77"/>
+      <c r="E30" s="77"/>
+      <c r="F30" s="77"/>
       <c r="G30" s="17"/>
       <c r="H30" s="17"/>
-      <c r="I30" s="69"/>
-      <c r="J30" s="69"/>
-      <c r="K30" s="69"/>
-      <c r="L30" s="69"/>
-      <c r="M30" s="69"/>
-      <c r="N30" s="69"/>
-      <c r="O30" s="69"/>
+      <c r="I30" s="77"/>
+      <c r="J30" s="77"/>
+      <c r="K30" s="77"/>
+      <c r="L30" s="77"/>
+      <c r="M30" s="77"/>
+      <c r="N30" s="77"/>
+      <c r="O30" s="77"/>
     </row>
     <row r="31" spans="1:15" ht="12.75" customHeight="1">
-      <c r="A31" s="93"/>
-      <c r="B31" s="94"/>
-      <c r="C31" s="95"/>
-      <c r="D31" s="99"/>
-      <c r="E31" s="98"/>
-      <c r="F31" s="98"/>
+      <c r="A31" s="90"/>
+      <c r="B31" s="92"/>
+      <c r="C31" s="93"/>
+      <c r="D31" s="94"/>
+      <c r="E31" s="95"/>
+      <c r="F31" s="95"/>
       <c r="G31" s="17"/>
       <c r="H31" s="17"/>
-      <c r="I31" s="70"/>
-      <c r="J31" s="86"/>
-      <c r="K31" s="70"/>
-      <c r="L31" s="70"/>
-      <c r="M31" s="70"/>
-      <c r="N31" s="70"/>
-      <c r="O31" s="70"/>
+      <c r="I31" s="81"/>
+      <c r="J31" s="88"/>
+      <c r="K31" s="81"/>
+      <c r="L31" s="81"/>
+      <c r="M31" s="81"/>
+      <c r="N31" s="81"/>
+      <c r="O31" s="81"/>
     </row>
     <row r="32" spans="1:15" ht="12.75" customHeight="1">
-      <c r="A32" s="88"/>
-      <c r="B32" s="88"/>
-      <c r="C32" s="88"/>
-      <c r="D32" s="88"/>
-      <c r="E32" s="88"/>
-      <c r="F32" s="88"/>
+      <c r="A32" s="91"/>
+      <c r="B32" s="91"/>
+      <c r="C32" s="91"/>
+      <c r="D32" s="91"/>
+      <c r="E32" s="91"/>
+      <c r="F32" s="91"/>
       <c r="G32" s="17"/>
       <c r="H32" s="17"/>
-      <c r="I32" s="88"/>
-      <c r="J32" s="88"/>
-      <c r="K32" s="88"/>
-      <c r="L32" s="88"/>
-      <c r="M32" s="88"/>
-      <c r="N32" s="88"/>
-      <c r="O32" s="88"/>
+      <c r="I32" s="91"/>
+      <c r="J32" s="91"/>
+      <c r="K32" s="91"/>
+      <c r="L32" s="91"/>
+      <c r="M32" s="91"/>
+      <c r="N32" s="91"/>
+      <c r="O32" s="91"/>
     </row>
     <row r="33" spans="1:15" ht="12.75" customHeight="1">
-      <c r="A33" s="88"/>
-      <c r="B33" s="88"/>
-      <c r="C33" s="88"/>
-      <c r="D33" s="88"/>
-      <c r="E33" s="88"/>
-      <c r="F33" s="88"/>
+      <c r="A33" s="91"/>
+      <c r="B33" s="91"/>
+      <c r="C33" s="91"/>
+      <c r="D33" s="91"/>
+      <c r="E33" s="91"/>
+      <c r="F33" s="91"/>
       <c r="G33" s="17"/>
       <c r="H33" s="17"/>
-      <c r="I33" s="88"/>
-      <c r="J33" s="88"/>
-      <c r="K33" s="88"/>
-      <c r="L33" s="88"/>
-      <c r="M33" s="88"/>
-      <c r="N33" s="88"/>
-      <c r="O33" s="88"/>
+      <c r="I33" s="91"/>
+      <c r="J33" s="91"/>
+      <c r="K33" s="91"/>
+      <c r="L33" s="91"/>
+      <c r="M33" s="91"/>
+      <c r="N33" s="91"/>
+      <c r="O33" s="91"/>
     </row>
     <row r="34" spans="1:15" ht="12.75" customHeight="1">
-      <c r="A34" s="69"/>
-      <c r="B34" s="69"/>
-      <c r="C34" s="69"/>
-      <c r="D34" s="69"/>
-      <c r="E34" s="69"/>
-      <c r="F34" s="69"/>
+      <c r="A34" s="77"/>
+      <c r="B34" s="77"/>
+      <c r="C34" s="77"/>
+      <c r="D34" s="77"/>
+      <c r="E34" s="77"/>
+      <c r="F34" s="77"/>
       <c r="G34" s="17"/>
       <c r="H34" s="17"/>
-      <c r="I34" s="69"/>
-      <c r="J34" s="69"/>
-      <c r="K34" s="69"/>
-      <c r="L34" s="69"/>
-      <c r="M34" s="69"/>
-      <c r="N34" s="69"/>
-      <c r="O34" s="69"/>
+      <c r="I34" s="77"/>
+      <c r="J34" s="77"/>
+      <c r="K34" s="77"/>
+      <c r="L34" s="77"/>
+      <c r="M34" s="77"/>
+      <c r="N34" s="77"/>
+      <c r="O34" s="77"/>
     </row>
     <row r="35" spans="1:15" ht="12.75" customHeight="1">
       <c r="E35" s="40"/>
@@ -53241,25 +53252,65 @@
     <row r="1000" ht="12.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="122">
-    <mergeCell ref="A31:A34"/>
-    <mergeCell ref="B31:B34"/>
-    <mergeCell ref="C31:C34"/>
-    <mergeCell ref="D31:D34"/>
-    <mergeCell ref="E31:E34"/>
-    <mergeCell ref="F31:F34"/>
-    <mergeCell ref="I31:I34"/>
-    <mergeCell ref="J8:J11"/>
-    <mergeCell ref="K8:K11"/>
-    <mergeCell ref="L8:L11"/>
-    <mergeCell ref="M8:M11"/>
-    <mergeCell ref="N8:N11"/>
-    <mergeCell ref="O8:O11"/>
-    <mergeCell ref="J31:J34"/>
-    <mergeCell ref="K31:K34"/>
-    <mergeCell ref="L31:L34"/>
-    <mergeCell ref="M31:M34"/>
-    <mergeCell ref="N31:N34"/>
-    <mergeCell ref="O31:O34"/>
+    <mergeCell ref="G9:G11"/>
+    <mergeCell ref="H9:H11"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="B8:B11"/>
+    <mergeCell ref="C8:C11"/>
+    <mergeCell ref="D8:D11"/>
+    <mergeCell ref="E8:E11"/>
+    <mergeCell ref="F8:F11"/>
+    <mergeCell ref="I8:I11"/>
+    <mergeCell ref="J12:J14"/>
+    <mergeCell ref="K12:K14"/>
+    <mergeCell ref="L12:L14"/>
+    <mergeCell ref="M12:M14"/>
+    <mergeCell ref="N12:N14"/>
+    <mergeCell ref="O12:O14"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="D12:D14"/>
+    <mergeCell ref="E12:E14"/>
+    <mergeCell ref="F12:F14"/>
+    <mergeCell ref="I12:I14"/>
+    <mergeCell ref="K15:K17"/>
+    <mergeCell ref="L15:L17"/>
+    <mergeCell ref="M15:M17"/>
+    <mergeCell ref="N15:N17"/>
+    <mergeCell ref="O15:O17"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="D15:D17"/>
+    <mergeCell ref="E15:E17"/>
+    <mergeCell ref="F15:F17"/>
+    <mergeCell ref="I15:I17"/>
+    <mergeCell ref="L18:L21"/>
+    <mergeCell ref="M18:M21"/>
+    <mergeCell ref="N18:N21"/>
+    <mergeCell ref="O18:O21"/>
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="C18:C21"/>
+    <mergeCell ref="D18:D21"/>
+    <mergeCell ref="E18:E21"/>
+    <mergeCell ref="F18:F21"/>
+    <mergeCell ref="I18:I21"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="N1:N2"/>
+    <mergeCell ref="O1:O2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="G1:H1"/>
     <mergeCell ref="J3:J7"/>
     <mergeCell ref="K3:K7"/>
     <mergeCell ref="L3:L7"/>
@@ -53275,26 +53326,39 @@
     <mergeCell ref="E3:E7"/>
     <mergeCell ref="F3:F7"/>
     <mergeCell ref="I3:I7"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="J1:J2"/>
-    <mergeCell ref="K1:K2"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="M1:M2"/>
-    <mergeCell ref="N1:N2"/>
-    <mergeCell ref="O1:O2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="L8:L11"/>
+    <mergeCell ref="M8:M11"/>
+    <mergeCell ref="N8:N11"/>
+    <mergeCell ref="O8:O11"/>
+    <mergeCell ref="J31:J34"/>
+    <mergeCell ref="K31:K34"/>
+    <mergeCell ref="L31:L34"/>
+    <mergeCell ref="M31:M34"/>
+    <mergeCell ref="N31:N34"/>
+    <mergeCell ref="O31:O34"/>
     <mergeCell ref="J27:J30"/>
     <mergeCell ref="K27:K30"/>
     <mergeCell ref="L27:L30"/>
     <mergeCell ref="M27:M30"/>
     <mergeCell ref="N27:N30"/>
     <mergeCell ref="O27:O30"/>
+    <mergeCell ref="J22:J26"/>
+    <mergeCell ref="K22:K26"/>
+    <mergeCell ref="L22:L26"/>
+    <mergeCell ref="M22:M26"/>
+    <mergeCell ref="N22:N26"/>
+    <mergeCell ref="O22:O26"/>
+    <mergeCell ref="J18:J21"/>
+    <mergeCell ref="K18:K21"/>
+    <mergeCell ref="A31:A34"/>
+    <mergeCell ref="B31:B34"/>
+    <mergeCell ref="C31:C34"/>
+    <mergeCell ref="D31:D34"/>
+    <mergeCell ref="E31:E34"/>
+    <mergeCell ref="F31:F34"/>
+    <mergeCell ref="I31:I34"/>
+    <mergeCell ref="J8:J11"/>
+    <mergeCell ref="K8:K11"/>
     <mergeCell ref="A27:A30"/>
     <mergeCell ref="B27:B30"/>
     <mergeCell ref="C27:C30"/>
@@ -53302,12 +53366,6 @@
     <mergeCell ref="E27:E30"/>
     <mergeCell ref="F27:F30"/>
     <mergeCell ref="I27:I30"/>
-    <mergeCell ref="J22:J26"/>
-    <mergeCell ref="K22:K26"/>
-    <mergeCell ref="L22:L26"/>
-    <mergeCell ref="M22:M26"/>
-    <mergeCell ref="N22:N26"/>
-    <mergeCell ref="O22:O26"/>
     <mergeCell ref="A22:A26"/>
     <mergeCell ref="B22:B26"/>
     <mergeCell ref="C22:C26"/>
@@ -53315,63 +53373,16 @@
     <mergeCell ref="E22:E26"/>
     <mergeCell ref="F22:F26"/>
     <mergeCell ref="I22:I26"/>
-    <mergeCell ref="J18:J21"/>
-    <mergeCell ref="K18:K21"/>
-    <mergeCell ref="L18:L21"/>
-    <mergeCell ref="M18:M21"/>
-    <mergeCell ref="N18:N21"/>
-    <mergeCell ref="O18:O21"/>
-    <mergeCell ref="A18:A21"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="C18:C21"/>
-    <mergeCell ref="D18:D21"/>
-    <mergeCell ref="E18:E21"/>
-    <mergeCell ref="F18:F21"/>
-    <mergeCell ref="I18:I21"/>
     <mergeCell ref="J15:J17"/>
-    <mergeCell ref="K15:K17"/>
-    <mergeCell ref="L15:L17"/>
-    <mergeCell ref="M15:M17"/>
-    <mergeCell ref="N15:N17"/>
-    <mergeCell ref="O15:O17"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="D15:D17"/>
-    <mergeCell ref="E15:E17"/>
-    <mergeCell ref="F15:F17"/>
-    <mergeCell ref="I15:I17"/>
-    <mergeCell ref="J12:J14"/>
-    <mergeCell ref="K12:K14"/>
-    <mergeCell ref="L12:L14"/>
-    <mergeCell ref="M12:M14"/>
-    <mergeCell ref="N12:N14"/>
-    <mergeCell ref="O12:O14"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="C12:C14"/>
-    <mergeCell ref="D12:D14"/>
-    <mergeCell ref="E12:E14"/>
-    <mergeCell ref="F12:F14"/>
-    <mergeCell ref="I12:I14"/>
-    <mergeCell ref="G9:G11"/>
-    <mergeCell ref="H9:H11"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="B8:B11"/>
-    <mergeCell ref="C8:C11"/>
-    <mergeCell ref="D8:D11"/>
-    <mergeCell ref="E8:E11"/>
-    <mergeCell ref="F8:F11"/>
-    <mergeCell ref="I8:I11"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" sqref="J3 J8 J12 J15 J18 J22 J27 J31" xr:uid="{00000000-0002-0000-0400-000000000000}">
+    <dataValidation type="list" allowBlank="1" sqref="J3 J8 J12 J15 J18 J22 J27 J31">
       <formula1>"Reportado,En revisión,Finalizado"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="O3" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
-    <hyperlink ref="O8" r:id="rId2" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
+    <hyperlink ref="O3" r:id="rId1"/>
+    <hyperlink ref="O8" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -53379,65 +53390,65 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="10.59765625" customWidth="1"/>
-    <col min="2" max="2" width="14.59765625" customWidth="1"/>
-    <col min="3" max="3" width="19.1328125" customWidth="1"/>
-    <col min="4" max="4" width="17.3984375" customWidth="1"/>
-    <col min="5" max="5" width="10.59765625" customWidth="1"/>
-    <col min="6" max="6" width="24.46484375" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" customWidth="1"/>
+    <col min="6" max="6" width="24.42578125" customWidth="1"/>
     <col min="7" max="7" width="25" customWidth="1"/>
-    <col min="8" max="8" width="10.59765625" customWidth="1"/>
-    <col min="9" max="9" width="51.59765625" customWidth="1"/>
-    <col min="10" max="26" width="10.59765625" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" customWidth="1"/>
+    <col min="9" max="9" width="51.5703125" customWidth="1"/>
+    <col min="10" max="26" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="33.75" customHeight="1">
       <c r="A1" s="54" t="s">
+        <v>643</v>
+      </c>
+      <c r="B1" s="54" t="s">
+        <v>644</v>
+      </c>
+      <c r="C1" s="54" t="s">
         <v>645</v>
-      </c>
-      <c r="B1" s="54" t="s">
-        <v>646</v>
-      </c>
-      <c r="C1" s="54" t="s">
-        <v>647</v>
       </c>
       <c r="D1" s="54" t="s">
         <v>7</v>
       </c>
       <c r="E1" s="54" t="s">
+        <v>646</v>
+      </c>
+      <c r="F1" s="54" t="s">
+        <v>647</v>
+      </c>
+      <c r="G1" s="54" t="s">
         <v>648</v>
       </c>
-      <c r="F1" s="54" t="s">
+      <c r="H1" s="54" t="s">
         <v>649</v>
       </c>
-      <c r="G1" s="54" t="s">
-        <v>650</v>
-      </c>
-      <c r="H1" s="54" t="s">
-        <v>651</v>
-      </c>
       <c r="I1" s="55" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="40.5" customHeight="1">
       <c r="A2" s="13" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="B2" s="56">
         <v>1</v>
       </c>
       <c r="C2" s="56" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="D2" s="13" t="s">
         <v>568</v>
@@ -53449,24 +53460,24 @@
         <v>292</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="H2" s="13" t="s">
         <v>202</v>
       </c>
       <c r="I2" s="57" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="40.5" customHeight="1">
       <c r="A3" s="13" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="B3" s="56">
         <v>1</v>
       </c>
       <c r="C3" s="56" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="D3" s="13" t="s">
         <v>568</v>
@@ -53478,24 +53489,24 @@
         <v>292</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="H3" s="13" t="s">
         <v>202</v>
       </c>
       <c r="I3" s="57" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="40.5" customHeight="1">
       <c r="A4" s="13" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="B4" s="56">
         <v>1</v>
       </c>
       <c r="C4" s="56" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="D4" s="13" t="s">
         <v>568</v>
@@ -53507,24 +53518,24 @@
         <v>292</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="H4" s="13" t="s">
         <v>202</v>
       </c>
       <c r="I4" s="57" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="40.5" customHeight="1">
       <c r="A5" s="13" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="B5" s="56">
         <v>1</v>
       </c>
       <c r="C5" s="56" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="D5" s="13" t="s">
         <v>568</v>
@@ -53536,24 +53547,24 @@
         <v>292</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="H5" s="13" t="s">
         <v>202</v>
       </c>
       <c r="I5" s="57" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="40.5" customHeight="1">
       <c r="A6" s="13" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="B6" s="56">
         <v>1</v>
       </c>
       <c r="C6" s="56" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="D6" s="13" t="s">
         <v>568</v>
@@ -53565,24 +53576,24 @@
         <v>292</v>
       </c>
       <c r="G6" s="13" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="H6" s="13" t="s">
         <v>202</v>
       </c>
       <c r="I6" s="57" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="66.75" customHeight="1">
       <c r="A7" s="13" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="B7" s="56">
         <v>1</v>
       </c>
       <c r="C7" s="56" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="D7" s="13" t="s">
         <v>568</v>
@@ -53594,24 +53605,24 @@
         <v>292</v>
       </c>
       <c r="G7" s="13" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="H7" s="13" t="s">
         <v>202</v>
       </c>
       <c r="I7" s="57" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="40.5" customHeight="1">
       <c r="A8" s="13" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="B8" s="56">
         <v>1</v>
       </c>
       <c r="C8" s="56" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="D8" s="13" t="s">
         <v>568</v>
@@ -53623,13 +53634,13 @@
         <v>292</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="H8" s="13" t="s">
         <v>202</v>
       </c>
       <c r="I8" s="57" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="40.5" customHeight="1">
@@ -53645,13 +53656,13 @@
     </row>
     <row r="10" spans="1:9" ht="40.5" customHeight="1">
       <c r="A10" s="13" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="B10" s="13">
         <v>2</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="D10" s="13" t="s">
         <v>568</v>
@@ -53661,24 +53672,24 @@
       </c>
       <c r="F10" s="13"/>
       <c r="G10" s="13" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="H10" s="13" t="s">
         <v>202</v>
       </c>
       <c r="I10" s="57" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="84.75" customHeight="1">
       <c r="A11" s="13" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="B11" s="13">
         <v>2</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="D11" s="13" t="s">
         <v>568</v>
@@ -53690,24 +53701,24 @@
         <v>292</v>
       </c>
       <c r="G11" s="13" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="H11" s="13" t="s">
         <v>202</v>
       </c>
       <c r="I11" s="57" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="83.25" customHeight="1">
       <c r="A12" s="13" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="B12" s="13">
         <v>2</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="D12" s="13" t="s">
         <v>568</v>
@@ -53719,24 +53730,24 @@
         <v>292</v>
       </c>
       <c r="G12" s="13" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="H12" s="13" t="s">
         <v>202</v>
       </c>
       <c r="I12" s="57" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="40.5" customHeight="1">
       <c r="A13" s="13" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="B13" s="13">
         <v>2</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="D13" s="13" t="s">
         <v>568</v>
@@ -53748,24 +53759,24 @@
         <v>292</v>
       </c>
       <c r="G13" s="13" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="H13" s="13" t="s">
         <v>202</v>
       </c>
       <c r="I13" s="57" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="69.75" customHeight="1">
       <c r="A14" s="13" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="B14" s="13">
         <v>2</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="D14" s="13" t="s">
         <v>568</v>
@@ -53777,24 +53788,24 @@
         <v>292</v>
       </c>
       <c r="G14" s="13" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="H14" s="13" t="s">
         <v>202</v>
       </c>
       <c r="I14" s="57" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="87" customHeight="1">
       <c r="A15" s="13" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="B15" s="13">
         <v>2</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="D15" s="13" t="s">
         <v>568</v>
@@ -53806,24 +53817,24 @@
         <v>292</v>
       </c>
       <c r="G15" s="13" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="H15" s="13" t="s">
         <v>202</v>
       </c>
       <c r="I15" s="57" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="78.75" customHeight="1">
       <c r="A16" s="13" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="B16" s="13">
         <v>2</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="D16" s="13" t="s">
         <v>568</v>
@@ -53835,24 +53846,24 @@
         <v>292</v>
       </c>
       <c r="G16" s="13" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="H16" s="13" t="s">
         <v>202</v>
       </c>
       <c r="I16" s="57" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="72.75" customHeight="1">
       <c r="A17" s="13" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="B17" s="13">
         <v>2</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="D17" s="13" t="s">
         <v>568</v>
@@ -53864,13 +53875,13 @@
         <v>292</v>
       </c>
       <c r="G17" s="13" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="H17" s="13" t="s">
         <v>202</v>
       </c>
       <c r="I17" s="57" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="40.5" customHeight="1">
@@ -53885,119 +53896,119 @@
       <c r="I18" s="59"/>
     </row>
     <row r="19" spans="1:9" ht="63.75">
-      <c r="A19" s="108" t="s">
+      <c r="A19" s="61" t="s">
+        <v>683</v>
+      </c>
+      <c r="B19" s="61">
+        <v>3</v>
+      </c>
+      <c r="C19" s="61" t="s">
+        <v>684</v>
+      </c>
+      <c r="D19" s="61" t="s">
+        <v>568</v>
+      </c>
+      <c r="E19" s="62">
+        <v>44782</v>
+      </c>
+      <c r="F19" s="61" t="s">
+        <v>292</v>
+      </c>
+      <c r="G19" s="61" t="s">
+        <v>652</v>
+      </c>
+      <c r="H19" s="61" t="s">
+        <v>202</v>
+      </c>
+      <c r="I19" s="63" t="s">
         <v>685</v>
       </c>
-      <c r="B19" s="108">
+    </row>
+    <row r="20" spans="1:9" ht="63.75">
+      <c r="A20" s="61" t="s">
+        <v>686</v>
+      </c>
+      <c r="B20" s="61">
         <v>3</v>
       </c>
-      <c r="C19" s="108" t="s">
-        <v>686</v>
-      </c>
-      <c r="D19" s="108" t="s">
+      <c r="C20" s="61" t="s">
+        <v>687</v>
+      </c>
+      <c r="D20" s="61" t="s">
         <v>568</v>
       </c>
-      <c r="E19" s="109">
+      <c r="E20" s="62">
         <v>44782</v>
       </c>
-      <c r="F19" s="108" t="s">
+      <c r="F20" s="61" t="s">
         <v>292</v>
       </c>
-      <c r="G19" s="108" t="s">
-        <v>654</v>
-      </c>
-      <c r="H19" s="108" t="s">
+      <c r="G20" s="61" t="s">
+        <v>652</v>
+      </c>
+      <c r="H20" s="61" t="s">
         <v>202</v>
       </c>
-      <c r="I19" s="110" t="s">
-        <v>687</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="63.75">
-      <c r="A20" s="108" t="s">
+      <c r="I20" s="63" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="76.5">
+      <c r="A21" s="61" t="s">
         <v>688</v>
       </c>
-      <c r="B20" s="108">
+      <c r="B21" s="61">
         <v>3</v>
       </c>
-      <c r="C20" s="108" t="s">
+      <c r="C21" s="61" t="s">
         <v>689</v>
       </c>
-      <c r="D20" s="108" t="s">
+      <c r="D21" s="61" t="s">
         <v>568</v>
       </c>
-      <c r="E20" s="109">
+      <c r="E21" s="62">
         <v>44782</v>
       </c>
-      <c r="F20" s="108" t="s">
+      <c r="F21" s="61" t="s">
         <v>292</v>
       </c>
-      <c r="G20" s="108" t="s">
-        <v>654</v>
-      </c>
-      <c r="H20" s="108" t="s">
+      <c r="G21" s="61" t="s">
+        <v>652</v>
+      </c>
+      <c r="H21" s="61" t="s">
         <v>202</v>
       </c>
-      <c r="I20" s="110" t="s">
-        <v>687</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="76.5">
-      <c r="A21" s="108" t="s">
+      <c r="I21" s="63" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="63.75">
+      <c r="A22" s="61" t="s">
         <v>690</v>
       </c>
-      <c r="B21" s="108">
+      <c r="B22" s="61">
         <v>3</v>
       </c>
-      <c r="C21" s="108" t="s">
+      <c r="C22" s="61" t="s">
         <v>691</v>
       </c>
-      <c r="D21" s="108" t="s">
+      <c r="D22" s="61" t="s">
         <v>568</v>
       </c>
-      <c r="E21" s="109">
+      <c r="E22" s="62">
         <v>44782</v>
       </c>
-      <c r="F21" s="108" t="s">
+      <c r="F22" s="61" t="s">
         <v>292</v>
       </c>
-      <c r="G21" s="108" t="s">
-        <v>654</v>
-      </c>
-      <c r="H21" s="108" t="s">
+      <c r="G22" s="61" t="s">
+        <v>652</v>
+      </c>
+      <c r="H22" s="61" t="s">
         <v>202</v>
       </c>
-      <c r="I21" s="110" t="s">
-        <v>687</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="63.75">
-      <c r="A22" s="108" t="s">
-        <v>692</v>
-      </c>
-      <c r="B22" s="108">
-        <v>3</v>
-      </c>
-      <c r="C22" s="108" t="s">
-        <v>693</v>
-      </c>
-      <c r="D22" s="108" t="s">
-        <v>568</v>
-      </c>
-      <c r="E22" s="109">
-        <v>44782</v>
-      </c>
-      <c r="F22" s="108" t="s">
-        <v>292</v>
-      </c>
-      <c r="G22" s="108" t="s">
-        <v>654</v>
-      </c>
-      <c r="H22" s="108" t="s">
-        <v>202</v>
-      </c>
-      <c r="I22" s="110" t="s">
-        <v>687</v>
+      <c r="I22" s="63" t="s">
+        <v>685</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="12.75" customHeight="1">
@@ -54990,25 +55001,25 @@
     <row r="1000" ht="12.75" customHeight="1"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
-    <hyperlink ref="I3" r:id="rId2" xr:uid="{00000000-0004-0000-0500-000001000000}"/>
-    <hyperlink ref="I4" r:id="rId3" xr:uid="{00000000-0004-0000-0500-000002000000}"/>
-    <hyperlink ref="I5" r:id="rId4" xr:uid="{00000000-0004-0000-0500-000003000000}"/>
-    <hyperlink ref="I6" r:id="rId5" xr:uid="{00000000-0004-0000-0500-000004000000}"/>
-    <hyperlink ref="I7" r:id="rId6" xr:uid="{00000000-0004-0000-0500-000005000000}"/>
-    <hyperlink ref="I8" r:id="rId7" xr:uid="{00000000-0004-0000-0500-000006000000}"/>
-    <hyperlink ref="I10" r:id="rId8" xr:uid="{00000000-0004-0000-0500-000007000000}"/>
-    <hyperlink ref="I11" r:id="rId9" xr:uid="{00000000-0004-0000-0500-000008000000}"/>
-    <hyperlink ref="I12" r:id="rId10" xr:uid="{00000000-0004-0000-0500-000009000000}"/>
-    <hyperlink ref="I13" r:id="rId11" xr:uid="{00000000-0004-0000-0500-00000A000000}"/>
-    <hyperlink ref="I14" r:id="rId12" xr:uid="{00000000-0004-0000-0500-00000B000000}"/>
-    <hyperlink ref="I15" r:id="rId13" xr:uid="{00000000-0004-0000-0500-00000C000000}"/>
-    <hyperlink ref="I16" r:id="rId14" xr:uid="{00000000-0004-0000-0500-00000D000000}"/>
-    <hyperlink ref="I17" r:id="rId15" xr:uid="{00000000-0004-0000-0500-00000E000000}"/>
-    <hyperlink ref="I19" r:id="rId16" xr:uid="{AE6F792D-D26A-47D2-8D3E-DEFFB4412C08}"/>
-    <hyperlink ref="I20" r:id="rId17" xr:uid="{5A0E887B-68AD-48F1-A613-B0B4E67858CB}"/>
-    <hyperlink ref="I21" r:id="rId18" xr:uid="{0B7B935A-C0B1-46DC-A37B-C801F51EF052}"/>
-    <hyperlink ref="I22" r:id="rId19" xr:uid="{75E7777F-1EC0-46F4-A66E-2D54F6B3B708}"/>
+    <hyperlink ref="I2" r:id="rId1"/>
+    <hyperlink ref="I3" r:id="rId2"/>
+    <hyperlink ref="I4" r:id="rId3"/>
+    <hyperlink ref="I5" r:id="rId4"/>
+    <hyperlink ref="I6" r:id="rId5"/>
+    <hyperlink ref="I7" r:id="rId6"/>
+    <hyperlink ref="I8" r:id="rId7"/>
+    <hyperlink ref="I10" r:id="rId8"/>
+    <hyperlink ref="I11" r:id="rId9"/>
+    <hyperlink ref="I12" r:id="rId10"/>
+    <hyperlink ref="I13" r:id="rId11"/>
+    <hyperlink ref="I14" r:id="rId12"/>
+    <hyperlink ref="I15" r:id="rId13"/>
+    <hyperlink ref="I16" r:id="rId14"/>
+    <hyperlink ref="I17" r:id="rId15"/>
+    <hyperlink ref="I19" r:id="rId16"/>
+    <hyperlink ref="I20" r:id="rId17"/>
+    <hyperlink ref="I21" r:id="rId18"/>
+    <hyperlink ref="I22" r:id="rId19"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId20"/>

</xml_diff>